<commit_message>
ancova with sociodemographic covar
</commit_message>
<xml_diff>
--- a/eg_data/NHANES/PF/Waist2/Demog/Demog.xlsx
+++ b/eg_data/NHANES/PF/Waist2/Demog/Demog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadoh\OneDrive\Documents\GitHub\DietR\eg_data\NHANES\PF\Waist2\Demog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5AF030-9128-4C87-A868-3BC46CED4EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417AA391-A3DF-4B15-8D27-51F3D540BCAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25155" yWindow="-3000" windowWidth="22230" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21660" yWindow="-3075" windowWidth="25290" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="32">
   <si>
     <t>Gender</t>
   </si>
@@ -130,6 +130,9 @@
   <si>
     <t>BEFORE REMOVING NA's in EDUCATION</t>
   </si>
+  <si>
+    <t>Horizontal %..  I don't think it's useful</t>
+  </si>
 </sst>
 </file>
 
@@ -208,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -234,12 +237,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -249,12 +246,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -271,15 +262,20 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -562,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Z63"/>
+  <dimension ref="B1:Z63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,28 +571,50 @@
     <col min="3" max="3" width="23.140625" customWidth="1"/>
     <col min="10" max="10" width="4.7109375" customWidth="1"/>
     <col min="11" max="11" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.28515625" customWidth="1"/>
     <col min="19" max="19" width="4.7109375" customWidth="1"/>
     <col min="20" max="20" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9.140625" style="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
     <row r="2" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>12</v>
+      <c r="L2" s="1" t="str">
+        <f>CONCATENATE("(n=",E7,")")</f>
+        <v>(n=1840)</v>
+      </c>
+      <c r="M2" s="1" t="str">
+        <f>CONCATENATE("(n=",F7,")")</f>
+        <v>(n=1114)</v>
+      </c>
+      <c r="N2" s="1" t="str">
+        <f>CONCATENATE("(n=",G7,")")</f>
+        <v>(n=361)</v>
+      </c>
+      <c r="O2" s="1" t="str">
+        <f>CONCATENATE("(n=",H7,")")</f>
+        <v>(n=361)</v>
       </c>
     </row>
     <row r="3" spans="2:26" x14ac:dyDescent="0.25">
@@ -617,13 +635,13 @@
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="11" t="s">
+      <c r="L3" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="Q3" s="4"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="U3" s="3" t="s">
@@ -659,26 +677,21 @@
       <c r="H4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="27" t="s">
+      <c r="J4" t="s">
         <v>0</v>
       </c>
-      <c r="K4" s="27"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27"/>
+      <c r="Q4" s="1"/>
       <c r="S4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="T4" s="4"/>
       <c r="U4" s="5"/>
-      <c r="V4" s="11" t="s">
+      <c r="V4" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="W4" s="12"/>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="12"/>
+      <c r="W4" s="25"/>
+      <c r="X4" s="25"/>
+      <c r="Y4" s="25"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
@@ -700,29 +713,28 @@
       <c r="H5" s="1">
         <v>172</v>
       </c>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27" t="s">
+      <c r="K5" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="26">
+      <c r="L5" s="7">
+        <f>E5/$E$7%</f>
+        <v>49.347826086956523</v>
+      </c>
+      <c r="M5" s="7">
+        <f>F5/$F$7%</f>
+        <v>45.691202872531413</v>
+      </c>
+      <c r="N5" s="7">
+        <f>G5/$G$7%</f>
+        <v>43.21329639889197</v>
+      </c>
+      <c r="O5" s="7">
+        <f>H5/$H$7%</f>
+        <v>47.64542936288089</v>
+      </c>
+      <c r="Q5" s="1">
         <f>IFERROR(D5,"")</f>
         <v>1745</v>
-      </c>
-      <c r="M5" s="28">
-        <f>E5/$E$7%</f>
-        <v>49.347826086956523</v>
-      </c>
-      <c r="N5" s="7">
-        <f>F5/$F$7%</f>
-        <v>45.691202872531413</v>
-      </c>
-      <c r="O5" s="7">
-        <f>G5/$G$7%</f>
-        <v>43.21329639889197</v>
-      </c>
-      <c r="P5" s="7">
-        <f>H5/$H$7%</f>
-        <v>47.64542936288089</v>
       </c>
       <c r="S5" s="2"/>
       <c r="T5" s="2" t="s">
@@ -775,25 +787,25 @@
       <c r="K6" t="s">
         <v>2</v>
       </c>
-      <c r="L6" s="26">
+      <c r="L6" s="7">
+        <f>E6/$E$7%</f>
+        <v>50.652173913043484</v>
+      </c>
+      <c r="M6" s="7">
+        <f>F6/$F$7%</f>
+        <v>54.30879712746858</v>
+      </c>
+      <c r="N6" s="7">
+        <f>G6/$G$7%</f>
+        <v>56.786703601108037</v>
+      </c>
+      <c r="O6" s="7">
+        <f>H6/$H$7%</f>
+        <v>52.354570637119117</v>
+      </c>
+      <c r="Q6" s="1">
         <f>IFERROR(D6,"")</f>
         <v>1931</v>
-      </c>
-      <c r="M6" s="7">
-        <f>E6/$E$7%</f>
-        <v>50.652173913043484</v>
-      </c>
-      <c r="N6" s="7">
-        <f>F6/$F$7%</f>
-        <v>54.30879712746858</v>
-      </c>
-      <c r="O6" s="7">
-        <f>G6/$G$7%</f>
-        <v>56.786703601108037</v>
-      </c>
-      <c r="P6" s="7">
-        <f>H6/$H$7%</f>
-        <v>52.354570637119117</v>
       </c>
       <c r="T6" t="s">
         <v>2</v>
@@ -846,8 +858,8 @@
       <c r="J7" t="s">
         <v>13</v>
       </c>
-      <c r="L7" s="26"/>
-      <c r="N7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="Q7" s="1"/>
       <c r="S7" t="s">
         <v>13</v>
       </c>
@@ -879,25 +891,25 @@
       <c r="K8" t="s">
         <v>22</v>
       </c>
-      <c r="L8" s="26">
-        <f t="shared" ref="L8:L24" si="2">IFERROR(D8,"")</f>
-        <v>1320</v>
-      </c>
-      <c r="M8" s="7">
+      <c r="L8" s="7">
         <f>E8/$E$7%</f>
         <v>38.804347826086961</v>
       </c>
-      <c r="N8" s="7">
+      <c r="M8" s="7">
         <f>F8/$F$7%</f>
         <v>33.662477558348293</v>
       </c>
-      <c r="O8" s="7">
+      <c r="N8" s="7">
         <f>G8/$G$7%</f>
         <v>30.193905817174517</v>
       </c>
-      <c r="P8" s="7">
+      <c r="O8" s="7">
         <f>H8/$H$7%</f>
         <v>33.795013850415515</v>
+      </c>
+      <c r="Q8" s="1">
+        <f>IFERROR(D8,"")</f>
+        <v>1320</v>
       </c>
       <c r="T8" t="s">
         <v>22</v>
@@ -949,25 +961,25 @@
       <c r="K9" t="s">
         <v>23</v>
       </c>
-      <c r="L9" s="26">
-        <f t="shared" si="2"/>
-        <v>1190</v>
+      <c r="L9" s="7">
+        <f>E9/$E$7%</f>
+        <v>30.815217391304351</v>
       </c>
       <c r="M9" s="7">
-        <f t="shared" ref="M9" si="3">E9/$E$7%</f>
-        <v>30.815217391304351</v>
-      </c>
-      <c r="N9" s="7">
         <f>F9/$F$7%</f>
         <v>32.854578096947932</v>
       </c>
-      <c r="O9" s="7">
+      <c r="N9" s="7">
         <f>G9/$G$7%</f>
         <v>38.227146814404435</v>
       </c>
-      <c r="P9" s="7">
-        <f t="shared" ref="P9:P10" si="4">H9/$H$7%</f>
+      <c r="O9" s="7">
+        <f>H9/$H$7%</f>
         <v>32.963988919667592</v>
+      </c>
+      <c r="Q9" s="1">
+        <f>IFERROR(D9,"")</f>
+        <v>1190</v>
       </c>
       <c r="T9" t="s">
         <v>23</v>
@@ -1019,25 +1031,25 @@
       <c r="K10" t="s">
         <v>24</v>
       </c>
-      <c r="L10" s="26">
-        <f t="shared" si="2"/>
-        <v>1166</v>
-      </c>
-      <c r="M10" s="7">
+      <c r="L10" s="7">
         <f>E10/$E$7%</f>
         <v>30.380434782608699</v>
       </c>
-      <c r="N10" s="7">
+      <c r="M10" s="7">
         <f>F10/$F$7%</f>
         <v>33.482944344703768</v>
       </c>
-      <c r="O10" s="7">
+      <c r="N10" s="7">
         <f>G10/$G$7%</f>
         <v>31.578947368421055</v>
       </c>
-      <c r="P10" s="7">
-        <f t="shared" si="4"/>
+      <c r="O10" s="7">
+        <f>H10/$H$7%</f>
         <v>33.2409972299169</v>
+      </c>
+      <c r="Q10" s="1">
+        <f>IFERROR(D10,"")</f>
+        <v>1166</v>
       </c>
       <c r="T10" t="s">
         <v>24</v>
@@ -1076,23 +1088,23 @@
         <v>1840</v>
       </c>
       <c r="F11" s="10">
-        <f t="shared" ref="F11:H11" si="5">SUM(F8:F10)</f>
+        <f t="shared" ref="F11:H11" si="2">SUM(F8:F10)</f>
         <v>1114</v>
       </c>
       <c r="G11" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>361</v>
       </c>
       <c r="H11" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>361</v>
       </c>
       <c r="J11" t="s">
         <v>3</v>
       </c>
-      <c r="L11" s="26"/>
+      <c r="M11" s="7"/>
       <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
+      <c r="Q11" s="1"/>
       <c r="S11" t="s">
         <v>3</v>
       </c>
@@ -1124,25 +1136,25 @@
       <c r="K12" t="s">
         <v>25</v>
       </c>
-      <c r="L12" s="26">
-        <f t="shared" si="2"/>
-        <v>1092</v>
-      </c>
-      <c r="M12" s="7">
+      <c r="L12" s="7">
         <f>E12/$E$7%</f>
         <v>27.173913043478262</v>
       </c>
-      <c r="N12" s="7">
+      <c r="M12" s="7">
         <f>F12/$F$7%</f>
         <v>34.470377019748653</v>
       </c>
-      <c r="O12" s="7">
+      <c r="N12" s="7">
         <f>G12/$G$7%</f>
         <v>25.207756232686982</v>
       </c>
-      <c r="P12" s="7">
+      <c r="O12" s="7">
         <f>H12/$H$7%</f>
         <v>32.409972299168977</v>
+      </c>
+      <c r="Q12" s="1">
+        <f>IFERROR(D12,"")</f>
+        <v>1092</v>
       </c>
       <c r="T12" t="s">
         <v>25</v>
@@ -1194,25 +1206,25 @@
       <c r="K13" t="s">
         <v>4</v>
       </c>
-      <c r="L13" s="26">
-        <f t="shared" si="2"/>
-        <v>1328</v>
+      <c r="L13" s="7">
+        <f>E13/$E$7%</f>
+        <v>36.195652173913047</v>
       </c>
       <c r="M13" s="7">
-        <f t="shared" ref="M13" si="6">E13/$E$7%</f>
-        <v>36.195652173913047</v>
-      </c>
-      <c r="N13" s="7">
         <f>F13/$F$7%</f>
         <v>35.637342908438058</v>
       </c>
-      <c r="O13" s="7">
+      <c r="N13" s="7">
         <f>G13/$G$7%</f>
         <v>37.396121883656512</v>
       </c>
-      <c r="P13" s="7">
-        <f t="shared" ref="P13" si="7">H13/$H$7%</f>
+      <c r="O13" s="7">
+        <f>H13/$H$7%</f>
         <v>36.011080332409975</v>
+      </c>
+      <c r="Q13" s="1">
+        <f>IFERROR(D13,"")</f>
+        <v>1328</v>
       </c>
       <c r="T13" t="s">
         <v>4</v>
@@ -1264,25 +1276,25 @@
       <c r="K14" t="s">
         <v>5</v>
       </c>
-      <c r="L14" s="26">
-        <f t="shared" si="2"/>
-        <v>753</v>
-      </c>
-      <c r="M14" s="7">
+      <c r="L14" s="7">
         <f>E14/$E$7%</f>
         <v>25.978260869565219</v>
       </c>
-      <c r="N14" s="7">
+      <c r="M14" s="7">
         <f>F14/$F$7%</f>
         <v>17.504488330341111</v>
       </c>
-      <c r="O14" s="7">
+      <c r="N14" s="7">
         <f>G14/$G$7%</f>
         <v>12.742382271468145</v>
       </c>
-      <c r="P14" s="7">
+      <c r="O14" s="7">
         <f>H14/$H$7%</f>
         <v>9.418282548476455</v>
+      </c>
+      <c r="Q14" s="1">
+        <f>IFERROR(D14,"")</f>
+        <v>753</v>
       </c>
       <c r="T14" t="s">
         <v>5</v>
@@ -1334,25 +1346,25 @@
       <c r="K15" t="s">
         <v>6</v>
       </c>
-      <c r="L15" s="26">
-        <f t="shared" si="2"/>
-        <v>363</v>
+      <c r="L15" s="7">
+        <f>E15/$E$7%</f>
+        <v>6.2500000000000009</v>
       </c>
       <c r="M15" s="7">
-        <f t="shared" ref="M15" si="8">E15/$E$7%</f>
-        <v>6.2500000000000009</v>
-      </c>
-      <c r="N15" s="7">
         <f>F15/$F$7%</f>
         <v>8.5278276481149007</v>
       </c>
-      <c r="O15" s="7">
+      <c r="N15" s="7">
         <f>G15/$G$7%</f>
         <v>21.883656509695292</v>
       </c>
-      <c r="P15" s="7">
-        <f t="shared" ref="P15:P16" si="9">H15/$H$7%</f>
+      <c r="O15" s="7">
+        <f>H15/$H$7%</f>
         <v>20.498614958448755</v>
+      </c>
+      <c r="Q15" s="1">
+        <f>IFERROR(D15,"")</f>
+        <v>363</v>
       </c>
       <c r="T15" t="s">
         <v>6</v>
@@ -1404,25 +1416,25 @@
       <c r="K16" t="s">
         <v>14</v>
       </c>
-      <c r="L16" s="26">
-        <f t="shared" si="2"/>
-        <v>140</v>
-      </c>
-      <c r="M16" s="7">
+      <c r="L16" s="7">
         <f>E16/$E$7%</f>
         <v>4.4021739130434785</v>
       </c>
-      <c r="N16" s="7">
+      <c r="M16" s="7">
         <f>F16/$F$7%</f>
         <v>3.859964093357271</v>
       </c>
-      <c r="O16" s="7">
+      <c r="N16" s="7">
         <f>G16/$G$7%</f>
         <v>2.770083102493075</v>
       </c>
-      <c r="P16" s="7">
-        <f t="shared" si="9"/>
+      <c r="O16" s="7">
+        <f>H16/$H$7%</f>
         <v>1.662049861495845</v>
+      </c>
+      <c r="Q16" s="1">
+        <f>IFERROR(D16,"")</f>
+        <v>140</v>
       </c>
       <c r="T16" t="s">
         <v>14</v>
@@ -1461,23 +1473,23 @@
         <v>1840</v>
       </c>
       <c r="F17" s="10">
-        <f t="shared" ref="F17:H17" si="10">SUM(F12:F16)</f>
+        <f t="shared" ref="F17:H17" si="3">SUM(F12:F16)</f>
         <v>1114</v>
       </c>
       <c r="G17" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>361</v>
       </c>
       <c r="H17" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>361</v>
       </c>
       <c r="J17" t="s">
         <v>7</v>
       </c>
-      <c r="L17" s="26"/>
+      <c r="M17" s="7"/>
       <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
+      <c r="Q17" s="1"/>
       <c r="S17" t="s">
         <v>7</v>
       </c>
@@ -1509,25 +1521,25 @@
       <c r="K18" t="s">
         <v>15</v>
       </c>
-      <c r="L18" s="26">
-        <f t="shared" si="2"/>
-        <v>1638</v>
-      </c>
-      <c r="M18" s="7">
+      <c r="L18" s="7">
         <f>E18/$E$7%</f>
         <v>49.402173913043484</v>
       </c>
-      <c r="N18" s="7">
+      <c r="M18" s="7">
         <f>F18/$F$7%</f>
         <v>44.524236983842009</v>
       </c>
-      <c r="O18" s="7">
+      <c r="N18" s="7">
         <f>G18/$G$7%</f>
         <v>30.193905817174517</v>
       </c>
-      <c r="P18" s="7">
+      <c r="O18" s="7">
         <f>H18/$H$7%</f>
         <v>34.34903047091413</v>
+      </c>
+      <c r="Q18" s="1">
+        <f>IFERROR(D18,"")</f>
+        <v>1638</v>
       </c>
       <c r="T18" t="s">
         <v>15</v>
@@ -1579,25 +1591,25 @@
       <c r="K19" t="s">
         <v>17</v>
       </c>
-      <c r="L19" s="26">
-        <f t="shared" si="2"/>
-        <v>760</v>
-      </c>
-      <c r="M19" s="7">
+      <c r="L19" s="7">
         <f>E19/$E$7%</f>
         <v>21.358695652173914</v>
       </c>
-      <c r="N19" s="7">
+      <c r="M19" s="7">
         <f>F19/$F$7%</f>
         <v>20.017953321364452</v>
       </c>
-      <c r="O19" s="7">
+      <c r="N19" s="7">
         <f>G19/$G$7%</f>
         <v>23.26869806094183</v>
       </c>
-      <c r="P19" s="7">
+      <c r="O19" s="7">
         <f>H19/$H$7%</f>
         <v>16.62049861495845</v>
+      </c>
+      <c r="Q19" s="1">
+        <f>IFERROR(D19,"")</f>
+        <v>760</v>
       </c>
       <c r="T19" t="s">
         <v>17</v>
@@ -1649,25 +1661,25 @@
       <c r="K20" t="s">
         <v>16</v>
       </c>
-      <c r="L20" s="26">
+      <c r="L20" s="7">
+        <f>E20/$E$7%</f>
+        <v>29.239130434782609</v>
+      </c>
+      <c r="M20" s="7">
+        <f>F20/$F$7%</f>
+        <v>35.457809694793532</v>
+      </c>
+      <c r="N20" s="7">
+        <f>G20/$G$7%</f>
+        <v>46.53739612188366</v>
+      </c>
+      <c r="O20" s="7">
+        <f>H20/$H$7%</f>
+        <v>49.030470914127427</v>
+      </c>
+      <c r="Q20" s="1">
         <f>IFERROR(D20,"")</f>
         <v>1278</v>
-      </c>
-      <c r="M20" s="7">
-        <f t="shared" ref="M20" si="11">E20/$E$7%</f>
-        <v>29.239130434782609</v>
-      </c>
-      <c r="N20" s="7">
-        <f>F20/$F$7%</f>
-        <v>35.457809694793532</v>
-      </c>
-      <c r="O20" s="7">
-        <f>G20/$G$7%</f>
-        <v>46.53739612188366</v>
-      </c>
-      <c r="P20" s="7">
-        <f>H20/$H$7%</f>
-        <v>49.030470914127427</v>
       </c>
       <c r="T20" t="s">
         <v>16</v>
@@ -1720,9 +1732,9 @@
       <c r="J21" t="s">
         <v>8</v>
       </c>
-      <c r="L21" s="26"/>
+      <c r="M21" s="7"/>
       <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
+      <c r="Q21" s="1"/>
       <c r="S21" t="s">
         <v>8</v>
       </c>
@@ -1736,7 +1748,7 @@
         <v>19</v>
       </c>
       <c r="D22" s="10">
-        <f t="shared" ref="D22:D23" si="12">SUM(E22:H22)</f>
+        <f t="shared" ref="D22:D23" si="4">SUM(E22:H22)</f>
         <v>720</v>
       </c>
       <c r="E22">
@@ -1754,25 +1766,25 @@
       <c r="K22" t="s">
         <v>19</v>
       </c>
-      <c r="L22" s="26">
-        <f t="shared" si="2"/>
-        <v>720</v>
-      </c>
-      <c r="M22" s="7">
+      <c r="L22" s="7">
         <f>E22/$E$7%</f>
         <v>21.684782608695652</v>
       </c>
-      <c r="N22" s="7">
+      <c r="M22" s="7">
         <f>F22/$F$7%</f>
         <v>20.466786355475762</v>
       </c>
-      <c r="O22" s="7">
+      <c r="N22" s="7">
         <f>G22/$G$7%</f>
         <v>11.634349030470915</v>
       </c>
-      <c r="P22" s="7">
+      <c r="O22" s="7">
         <f>H22/$H$7%</f>
         <v>14.127423822714682</v>
+      </c>
+      <c r="Q22" s="1">
+        <f>IFERROR(D22,"")</f>
+        <v>720</v>
       </c>
       <c r="T22" t="s">
         <v>19</v>
@@ -1806,7 +1818,7 @@
         <v>21</v>
       </c>
       <c r="D23" s="10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="4"/>
         <v>1965</v>
       </c>
       <c r="E23">
@@ -1824,25 +1836,25 @@
       <c r="K23" t="s">
         <v>21</v>
       </c>
-      <c r="L23" s="26">
-        <f t="shared" si="2"/>
-        <v>1965</v>
-      </c>
-      <c r="M23" s="7">
+      <c r="L23" s="7">
         <f>E23/$E$7%</f>
         <v>58.586956521739133</v>
       </c>
-      <c r="N23" s="7">
+      <c r="M23" s="7">
         <f>F23/$F$7%</f>
         <v>51.526032315978455</v>
       </c>
-      <c r="O23" s="7">
+      <c r="N23" s="7">
         <f>G23/$G$7%</f>
         <v>44.598337950138507</v>
       </c>
-      <c r="P23" s="7">
-        <f t="shared" ref="P23" si="13">H23/$H$7%</f>
+      <c r="O23" s="7">
+        <f>H23/$H$7%</f>
         <v>42.10526315789474</v>
+      </c>
+      <c r="Q23" s="1">
+        <f>IFERROR(D23,"")</f>
+        <v>1965</v>
       </c>
       <c r="S23" s="4"/>
       <c r="T23" s="4" t="s">
@@ -1896,27 +1908,27 @@
       <c r="K24" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L24" s="5">
-        <f t="shared" si="2"/>
-        <v>991</v>
-      </c>
-      <c r="M24" s="8">
+      <c r="L24" s="8">
         <f>E24/$E$7%</f>
         <v>19.728260869565219</v>
       </c>
-      <c r="N24" s="8">
+      <c r="M24" s="8">
         <f>F24/$F$7%</f>
         <v>28.00718132854578</v>
       </c>
-      <c r="O24" s="8">
+      <c r="N24" s="8">
         <f>G24/$G$7%</f>
         <v>43.767313019390585</v>
       </c>
-      <c r="P24" s="8">
+      <c r="O24" s="8">
         <f>H24/$H$7%</f>
         <v>43.767313019390585</v>
       </c>
-      <c r="Q24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="5">
+        <f>IFERROR(D24,"")</f>
+        <v>991</v>
+      </c>
       <c r="T24" t="s">
         <v>20</v>
       </c>
@@ -1951,15 +1963,15 @@
         <v>1840</v>
       </c>
       <c r="F25" s="10">
-        <f t="shared" ref="F25:H25" si="14">SUM(F22:F24)</f>
+        <f t="shared" ref="F25:H25" si="5">SUM(F22:F24)</f>
         <v>1114</v>
       </c>
       <c r="G25" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>361</v>
       </c>
       <c r="H25" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>361</v>
       </c>
     </row>
@@ -1984,1443 +1996,1443 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="2:26" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="29" t="s">
+    <row r="29" spans="2:26" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="U29" s="30"/>
-    </row>
-    <row r="30" spans="2:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="14" t="s">
+      <c r="U29" s="23"/>
+    </row>
+    <row r="30" spans="2:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="E30" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F30" s="14" t="s">
+      <c r="F30" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G30" s="14" t="s">
+      <c r="G30" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H30" s="14" t="s">
+      <c r="H30" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="16" t="s">
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="M30" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="N30" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="O30" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q30" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="M30" s="16" t="s">
+      <c r="S30" s="13"/>
+      <c r="T30" s="13"/>
+      <c r="U30" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="V30" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="N30" s="16" t="s">
+      <c r="W30" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="O30" s="16" t="s">
+      <c r="X30" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="P30" s="16" t="s">
+      <c r="Y30" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="S30" s="15"/>
-      <c r="T30" s="15"/>
-      <c r="U30" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="V30" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="W30" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="X30" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y30" s="16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="2:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="13" t="s">
+    </row>
+    <row r="31" spans="2:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14" t="s">
+      <c r="D31" s="12"/>
+      <c r="E31" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F31" s="14" t="s">
+      <c r="F31" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="G31" s="14" t="s">
+      <c r="G31" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="H31" s="14" t="s">
+      <c r="H31" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="J31" s="17" t="s">
+      <c r="J31" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="K31" s="17"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="19" t="s">
+      <c r="K31" s="15"/>
+      <c r="L31" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="N31" s="20"/>
-      <c r="O31" s="20"/>
-      <c r="P31" s="20"/>
-      <c r="S31" s="17" t="s">
+      <c r="M31" s="27"/>
+      <c r="N31" s="27"/>
+      <c r="O31" s="27"/>
+      <c r="Q31" s="16"/>
+      <c r="S31" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="T31" s="17"/>
-      <c r="U31" s="18"/>
-      <c r="V31" s="19" t="s">
+      <c r="T31" s="15"/>
+      <c r="U31" s="16"/>
+      <c r="V31" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="W31" s="20"/>
-      <c r="X31" s="20"/>
-      <c r="Y31" s="20"/>
-    </row>
-    <row r="32" spans="2:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="13" t="s">
+      <c r="W31" s="27"/>
+      <c r="X31" s="27"/>
+      <c r="Y31" s="27"/>
+    </row>
+    <row r="32" spans="2:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D32" s="21">
+      <c r="D32" s="17">
         <f>SUM(E32:H32)</f>
         <v>1915</v>
       </c>
-      <c r="E32" s="14">
+      <c r="E32" s="12">
         <v>996</v>
       </c>
-      <c r="F32" s="14">
+      <c r="F32" s="12">
         <v>572</v>
       </c>
-      <c r="G32" s="14">
+      <c r="G32" s="12">
         <v>171</v>
       </c>
-      <c r="H32" s="14">
+      <c r="H32" s="12">
         <v>176</v>
       </c>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15" t="s">
+      <c r="J32" s="13"/>
+      <c r="K32" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="L32" s="16">
-        <v>1915</v>
-      </c>
-      <c r="M32" s="22">
+      <c r="L32" s="18">
         <f>E32/$E$7%</f>
         <v>54.130434782608702</v>
       </c>
-      <c r="N32" s="23">
+      <c r="M32" s="19">
         <f>F32/$F$7%</f>
         <v>51.346499102333929</v>
       </c>
-      <c r="O32" s="23">
+      <c r="N32" s="19">
         <f>G32/$G$7%</f>
         <v>47.368421052631582</v>
       </c>
-      <c r="P32" s="23">
+      <c r="O32" s="19">
         <f>H32/$H$7%</f>
         <v>48.75346260387812</v>
       </c>
-      <c r="S32" s="15"/>
-      <c r="T32" s="15" t="s">
+      <c r="Q32" s="14">
+        <v>1915</v>
+      </c>
+      <c r="S32" s="13"/>
+      <c r="T32" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="U32" s="16">
+      <c r="U32" s="14">
         <v>1915</v>
       </c>
-      <c r="V32" s="22">
+      <c r="V32" s="18">
         <f>E32/D32*100</f>
         <v>52.010443864229764</v>
       </c>
-      <c r="W32" s="22">
+      <c r="W32" s="18">
         <f>F32/D32*100</f>
         <v>29.869451697127936</v>
       </c>
-      <c r="X32" s="22">
+      <c r="X32" s="18">
         <f>G32/D32*100</f>
         <v>8.9295039164490859</v>
       </c>
-      <c r="Y32" s="22">
+      <c r="Y32" s="18">
         <f>H32/D32*100</f>
         <v>9.1906005221932112</v>
       </c>
-      <c r="Z32" s="24">
+      <c r="Z32" s="20">
         <f>SUM(V32:Y32)</f>
         <v>99.999999999999986</v>
       </c>
     </row>
-    <row r="33" spans="2:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C33" s="13" t="s">
+    <row r="33" spans="2:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C33" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D33" s="21">
+      <c r="D33" s="17">
         <f>SUM(E33:H33)</f>
         <v>2123</v>
       </c>
-      <c r="E33" s="14">
+      <c r="E33" s="12">
         <v>1016</v>
       </c>
-      <c r="F33" s="14">
+      <c r="F33" s="12">
         <v>674</v>
       </c>
-      <c r="G33" s="14">
+      <c r="G33" s="12">
         <v>216</v>
       </c>
-      <c r="H33" s="14">
+      <c r="H33" s="12">
         <v>217</v>
       </c>
-      <c r="K33" s="13" t="s">
+      <c r="K33" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="L33" s="14">
-        <v>2123</v>
-      </c>
-      <c r="M33" s="23">
+      <c r="L33" s="19">
         <f>E33/$E$7%</f>
         <v>55.217391304347828</v>
       </c>
-      <c r="N33" s="23">
+      <c r="M33" s="19">
         <f>F33/$F$7%</f>
         <v>60.502692998204665</v>
       </c>
-      <c r="O33" s="23">
+      <c r="N33" s="19">
         <f>G33/$G$7%</f>
         <v>59.83379501385042</v>
       </c>
-      <c r="P33" s="23">
+      <c r="O33" s="19">
         <f>H33/$H$7%</f>
         <v>60.110803324099727</v>
       </c>
-      <c r="T33" s="13" t="s">
+      <c r="Q33" s="12">
+        <v>2123</v>
+      </c>
+      <c r="T33" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="U33" s="14">
+      <c r="U33" s="12">
         <v>2123</v>
       </c>
-      <c r="V33" s="23">
+      <c r="V33" s="19">
         <f>E33/D33*100</f>
         <v>47.856806406029207</v>
       </c>
-      <c r="W33" s="23">
+      <c r="W33" s="19">
         <f>F33/D33*100</f>
         <v>31.747527084314648</v>
       </c>
-      <c r="X33" s="23">
+      <c r="X33" s="19">
         <f>G33/D33*100</f>
         <v>10.174281676872351</v>
       </c>
-      <c r="Y33" s="23">
+      <c r="Y33" s="19">
         <f>H33/D33*100</f>
         <v>10.221384832783796</v>
       </c>
-      <c r="Z33" s="24">
-        <f t="shared" ref="Z33:Z51" si="15">SUM(V33:Y33)</f>
+      <c r="Z33" s="20">
+        <f t="shared" ref="Z33:Z51" si="6">SUM(V33:Y33)</f>
         <v>100.00000000000001</v>
       </c>
     </row>
-    <row r="34" spans="2:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="13" t="s">
+    <row r="34" spans="2:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D34" s="14"/>
-      <c r="E34" s="21">
+      <c r="D34" s="12"/>
+      <c r="E34" s="17">
         <f>SUM(E32:E33)</f>
         <v>2012</v>
       </c>
-      <c r="F34" s="21">
-        <f t="shared" ref="F34:H34" si="16">SUM(F32:F33)</f>
+      <c r="F34" s="17">
+        <f t="shared" ref="F34:H34" si="7">SUM(F32:F33)</f>
         <v>1246</v>
       </c>
-      <c r="G34" s="21">
-        <f t="shared" si="16"/>
+      <c r="G34" s="17">
+        <f t="shared" si="7"/>
         <v>387</v>
       </c>
-      <c r="H34" s="21">
-        <f t="shared" si="16"/>
+      <c r="H34" s="17">
+        <f t="shared" si="7"/>
         <v>393</v>
       </c>
-      <c r="J34" s="13" t="s">
+      <c r="J34" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="L34" s="14"/>
-      <c r="N34" s="23"/>
-      <c r="S34" s="13" t="s">
+      <c r="M34" s="19"/>
+      <c r="Q34" s="12"/>
+      <c r="S34" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="U34" s="14"/>
-      <c r="Z34" s="24">
-        <f t="shared" si="15"/>
+      <c r="U34" s="12"/>
+      <c r="Z34" s="20">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="13" t="s">
+    <row r="35" spans="2:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C35" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D35" s="21">
+      <c r="D35" s="17">
         <f>SUM(E35:H35)</f>
         <v>1429</v>
       </c>
-      <c r="E35" s="14">
+      <c r="E35" s="12">
         <v>773</v>
       </c>
-      <c r="F35" s="14">
+      <c r="F35" s="12">
         <v>409</v>
       </c>
-      <c r="G35" s="14">
+      <c r="G35" s="12">
         <v>125</v>
       </c>
-      <c r="H35" s="14">
+      <c r="H35" s="12">
         <v>122</v>
       </c>
-      <c r="K35" s="13" t="s">
+      <c r="K35" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="L35" s="14">
-        <v>1429</v>
-      </c>
-      <c r="M35" s="23">
+      <c r="L35" s="19">
         <f>E35/$E$7%</f>
         <v>42.010869565217398</v>
       </c>
-      <c r="N35" s="23">
-        <f t="shared" ref="N35:N51" si="17">F35/$F$7%</f>
+      <c r="M35" s="19">
+        <f t="shared" ref="M35:M37" si="8">F35/$F$7%</f>
         <v>36.714542190305202</v>
       </c>
-      <c r="O35" s="23">
+      <c r="N35" s="19">
         <f>G35/$G$7%</f>
         <v>34.626038781163437</v>
       </c>
-      <c r="P35" s="23">
+      <c r="O35" s="19">
         <f>H35/$H$7%</f>
         <v>33.795013850415515</v>
       </c>
-      <c r="T35" s="13" t="s">
+      <c r="Q35" s="12">
+        <v>1429</v>
+      </c>
+      <c r="T35" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="U35" s="14">
+      <c r="U35" s="12">
         <v>1429</v>
       </c>
-      <c r="V35" s="23">
+      <c r="V35" s="19">
         <f>E35/D35*100</f>
         <v>54.093771868439468</v>
       </c>
-      <c r="W35" s="23">
+      <c r="W35" s="19">
         <f>F35/D35*100</f>
         <v>28.621413575927225</v>
       </c>
-      <c r="X35" s="23">
+      <c r="X35" s="19">
         <f>G35/D35*100</f>
         <v>8.7473757872638203</v>
       </c>
-      <c r="Y35" s="23">
+      <c r="Y35" s="19">
         <f>H35/D35*100</f>
         <v>8.5374387683694888</v>
       </c>
-      <c r="Z35" s="24">
-        <f t="shared" si="15"/>
+      <c r="Z35" s="20">
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="2:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="13" t="s">
+    <row r="36" spans="2:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C36" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D36" s="21">
+      <c r="D36" s="17">
         <f>SUM(E36:H36)</f>
         <v>1297</v>
       </c>
-      <c r="E36" s="14">
+      <c r="E36" s="12">
         <v>615</v>
       </c>
-      <c r="F36" s="14">
+      <c r="F36" s="12">
         <v>409</v>
       </c>
-      <c r="G36" s="14">
+      <c r="G36" s="12">
         <v>136</v>
       </c>
-      <c r="H36" s="14">
+      <c r="H36" s="12">
         <v>137</v>
       </c>
-      <c r="K36" s="13" t="s">
+      <c r="K36" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="L36" s="14">
-        <v>1297</v>
-      </c>
-      <c r="M36" s="23">
-        <f t="shared" ref="M36" si="18">E36/$E$7%</f>
+      <c r="L36" s="19">
+        <f t="shared" ref="L36" si="9">E36/$E$7%</f>
         <v>33.423913043478265</v>
       </c>
-      <c r="N36" s="23">
-        <f t="shared" si="17"/>
+      <c r="M36" s="19">
+        <f t="shared" si="8"/>
         <v>36.714542190305202</v>
       </c>
-      <c r="O36" s="23">
+      <c r="N36" s="19">
         <f>G36/$G$7%</f>
         <v>37.67313019390582</v>
       </c>
-      <c r="P36" s="23">
-        <f t="shared" ref="P36:P37" si="19">H36/$H$7%</f>
+      <c r="O36" s="19">
+        <f t="shared" ref="O36:O37" si="10">H36/$H$7%</f>
         <v>37.950138504155127</v>
       </c>
-      <c r="T36" s="13" t="s">
+      <c r="Q36" s="12">
+        <v>1297</v>
+      </c>
+      <c r="T36" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="U36" s="14">
+      <c r="U36" s="12">
         <v>1297</v>
       </c>
-      <c r="V36" s="23">
+      <c r="V36" s="19">
         <f>E36/D36*100</f>
         <v>47.417116422513494</v>
       </c>
-      <c r="W36" s="23">
+      <c r="W36" s="19">
         <f>F36/D36*100</f>
         <v>31.5343099460293</v>
       </c>
-      <c r="X36" s="23">
+      <c r="X36" s="19">
         <f>G36/D36*100</f>
         <v>10.485736314572089</v>
       </c>
-      <c r="Y36" s="23">
+      <c r="Y36" s="19">
         <f>H36/D36*100</f>
         <v>10.562837316885119</v>
       </c>
-      <c r="Z36" s="24">
-        <f t="shared" si="15"/>
+      <c r="Z36" s="20">
+        <f t="shared" si="6"/>
         <v>100.00000000000001</v>
       </c>
     </row>
-    <row r="37" spans="2:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="13" t="s">
+    <row r="37" spans="2:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="21">
+      <c r="D37" s="17">
         <f>SUM(E37:H37)</f>
         <v>1312</v>
       </c>
-      <c r="E37" s="14">
+      <c r="E37" s="12">
         <v>624</v>
       </c>
-      <c r="F37" s="14">
+      <c r="F37" s="12">
         <v>428</v>
       </c>
-      <c r="G37" s="14">
+      <c r="G37" s="12">
         <v>126</v>
       </c>
-      <c r="H37" s="14">
+      <c r="H37" s="12">
         <v>134</v>
       </c>
-      <c r="K37" s="13" t="s">
+      <c r="K37" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="L37" s="14">
-        <v>1312</v>
-      </c>
-      <c r="M37" s="23">
+      <c r="L37" s="19">
         <f>E37/$E$7%</f>
         <v>33.913043478260875</v>
       </c>
-      <c r="N37" s="23">
-        <f t="shared" si="17"/>
+      <c r="M37" s="19">
+        <f t="shared" si="8"/>
         <v>38.420107719928183</v>
       </c>
-      <c r="O37" s="23">
-        <f t="shared" ref="O37:O51" si="20">G37/$G$7%</f>
+      <c r="N37" s="19">
+        <f t="shared" ref="N37" si="11">G37/$G$7%</f>
         <v>34.903047091412745</v>
       </c>
-      <c r="P37" s="23">
-        <f t="shared" si="19"/>
+      <c r="O37" s="19">
+        <f t="shared" si="10"/>
         <v>37.119113573407205</v>
       </c>
-      <c r="T37" s="13" t="s">
+      <c r="Q37" s="12">
+        <v>1312</v>
+      </c>
+      <c r="T37" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="U37" s="14">
+      <c r="U37" s="12">
         <v>1312</v>
       </c>
-      <c r="V37" s="23">
+      <c r="V37" s="19">
         <f>E37/D37*100</f>
         <v>47.560975609756099</v>
       </c>
-      <c r="W37" s="23">
+      <c r="W37" s="19">
         <f>F37/D37*100</f>
         <v>32.621951219512198</v>
       </c>
-      <c r="X37" s="23">
+      <c r="X37" s="19">
         <f>G37/D37*100</f>
         <v>9.6036585365853657</v>
       </c>
-      <c r="Y37" s="23">
+      <c r="Y37" s="19">
         <f>H37/D37*100</f>
         <v>10.213414634146341</v>
       </c>
-      <c r="Z37" s="24">
-        <f t="shared" si="15"/>
+      <c r="Z37" s="20">
+        <f t="shared" si="6"/>
         <v>100.00000000000001</v>
       </c>
     </row>
-    <row r="38" spans="2:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="13" t="s">
+    <row r="38" spans="2:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D38" s="14"/>
-      <c r="E38" s="21">
+      <c r="D38" s="12"/>
+      <c r="E38" s="17">
         <f>SUM(E35:E37)</f>
         <v>2012</v>
       </c>
-      <c r="F38" s="21">
-        <f t="shared" ref="F38:H38" si="21">SUM(F35:F37)</f>
+      <c r="F38" s="17">
+        <f t="shared" ref="F38:H38" si="12">SUM(F35:F37)</f>
         <v>1246</v>
       </c>
-      <c r="G38" s="21">
-        <f t="shared" si="21"/>
+      <c r="G38" s="17">
+        <f t="shared" si="12"/>
         <v>387</v>
       </c>
-      <c r="H38" s="21">
-        <f t="shared" si="21"/>
+      <c r="H38" s="17">
+        <f t="shared" si="12"/>
         <v>393</v>
       </c>
-      <c r="J38" s="13" t="s">
+      <c r="J38" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="L38" s="14"/>
-      <c r="N38" s="23"/>
-      <c r="O38" s="23"/>
-      <c r="S38" s="13" t="s">
+      <c r="M38" s="19"/>
+      <c r="N38" s="19"/>
+      <c r="Q38" s="12"/>
+      <c r="S38" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="U38" s="14"/>
-      <c r="Z38" s="24">
-        <f t="shared" si="15"/>
+      <c r="U38" s="12"/>
+      <c r="Z38" s="20">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C39" s="13" t="s">
+    <row r="39" spans="2:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C39" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D39" s="21">
+      <c r="D39" s="17">
         <f>SUM(E39:H39)</f>
         <v>1210</v>
       </c>
-      <c r="E39" s="14">
+      <c r="E39" s="12">
         <v>545</v>
       </c>
-      <c r="F39" s="14">
+      <c r="F39" s="12">
         <v>438</v>
       </c>
-      <c r="G39" s="14">
+      <c r="G39" s="12">
         <v>108</v>
       </c>
-      <c r="H39" s="14">
+      <c r="H39" s="12">
         <v>119</v>
       </c>
-      <c r="K39" s="13" t="s">
+      <c r="K39" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="L39" s="14">
-        <v>1210</v>
-      </c>
-      <c r="M39" s="23">
+      <c r="L39" s="19">
         <f>E39/$E$7%</f>
         <v>29.619565217391308</v>
       </c>
-      <c r="N39" s="23">
-        <f t="shared" ref="N39:N53" si="22">F39/$F$7%</f>
+      <c r="M39" s="19">
+        <f t="shared" ref="M39:M43" si="13">F39/$F$7%</f>
         <v>39.317773788150809</v>
       </c>
-      <c r="O39" s="23">
-        <f t="shared" ref="O39:O53" si="23">G39/$G$7%</f>
+      <c r="N39" s="19">
+        <f t="shared" ref="N39:N43" si="14">G39/$G$7%</f>
         <v>29.91689750692521</v>
       </c>
-      <c r="P39" s="23">
+      <c r="O39" s="19">
         <f>H39/$H$7%</f>
         <v>32.963988919667592</v>
       </c>
-      <c r="T39" s="13" t="s">
+      <c r="Q39" s="12">
+        <v>1210</v>
+      </c>
+      <c r="T39" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="U39" s="14">
+      <c r="U39" s="12">
         <v>1210</v>
       </c>
-      <c r="V39" s="23">
+      <c r="V39" s="19">
         <f>E39/D39*100</f>
         <v>45.041322314049587</v>
       </c>
-      <c r="W39" s="23">
+      <c r="W39" s="19">
         <f>F39/D39*100</f>
         <v>36.198347107438018</v>
       </c>
-      <c r="X39" s="23">
+      <c r="X39" s="19">
         <f>G39/D39*100</f>
         <v>8.9256198347107443</v>
       </c>
-      <c r="Y39" s="23">
+      <c r="Y39" s="19">
         <f>H39/D39*100</f>
         <v>9.8347107438016526</v>
       </c>
-      <c r="Z39" s="24">
-        <f t="shared" si="15"/>
+      <c r="Z39" s="20">
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="2:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="13" t="s">
+    <row r="40" spans="2:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C40" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D40" s="21">
+      <c r="D40" s="17">
         <f>SUM(E40:H40)</f>
         <v>1410</v>
       </c>
-      <c r="E40" s="14">
+      <c r="E40" s="12">
         <v>708</v>
       </c>
-      <c r="F40" s="14">
+      <c r="F40" s="12">
         <v>426</v>
       </c>
-      <c r="G40" s="14">
+      <c r="G40" s="12">
         <v>134</v>
       </c>
-      <c r="H40" s="14">
+      <c r="H40" s="12">
         <v>142</v>
       </c>
-      <c r="K40" s="13" t="s">
+      <c r="K40" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="L40" s="14">
+      <c r="L40" s="19">
+        <f t="shared" ref="L40" si="15">E40/$E$7%</f>
+        <v>38.478260869565219</v>
+      </c>
+      <c r="M40" s="19">
+        <f t="shared" si="13"/>
+        <v>38.240574506283657</v>
+      </c>
+      <c r="N40" s="19">
+        <f t="shared" si="14"/>
+        <v>37.119113573407205</v>
+      </c>
+      <c r="O40" s="19">
+        <f t="shared" ref="O40" si="16">H40/$H$7%</f>
+        <v>39.335180055401665</v>
+      </c>
+      <c r="Q40" s="12">
         <v>1410</v>
       </c>
-      <c r="M40" s="23">
-        <f t="shared" ref="M40" si="24">E40/$E$7%</f>
-        <v>38.478260869565219</v>
-      </c>
-      <c r="N40" s="23">
-        <f t="shared" si="22"/>
-        <v>38.240574506283657</v>
-      </c>
-      <c r="O40" s="23">
-        <f t="shared" si="23"/>
-        <v>37.119113573407205</v>
-      </c>
-      <c r="P40" s="23">
-        <f t="shared" ref="P40" si="25">H40/$H$7%</f>
-        <v>39.335180055401665</v>
-      </c>
-      <c r="T40" s="13" t="s">
+      <c r="T40" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="U40" s="14">
+      <c r="U40" s="12">
         <v>1410</v>
       </c>
-      <c r="V40" s="23">
+      <c r="V40" s="19">
         <f>E40/D40*100</f>
         <v>50.212765957446805</v>
       </c>
-      <c r="W40" s="23">
+      <c r="W40" s="19">
         <f>F40/D40*100</f>
         <v>30.212765957446809</v>
       </c>
-      <c r="X40" s="23">
+      <c r="X40" s="19">
         <f>G40/D40*100</f>
         <v>9.5035460992907801</v>
       </c>
-      <c r="Y40" s="23">
+      <c r="Y40" s="19">
         <f>H40/D40*100</f>
         <v>10.070921985815604</v>
       </c>
-      <c r="Z40" s="24">
-        <f t="shared" si="15"/>
+      <c r="Z40" s="20">
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="2:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C41" s="13" t="s">
+    <row r="41" spans="2:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C41" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D41" s="21">
+      <c r="D41" s="17">
         <f>SUM(E41:H41)</f>
         <v>851</v>
       </c>
-      <c r="E41" s="14">
+      <c r="E41" s="12">
         <v>540</v>
       </c>
-      <c r="F41" s="14">
+      <c r="F41" s="12">
         <v>223</v>
       </c>
-      <c r="G41" s="14">
+      <c r="G41" s="12">
         <v>54</v>
       </c>
-      <c r="H41" s="14">
+      <c r="H41" s="12">
         <v>34</v>
       </c>
-      <c r="K41" s="13" t="s">
+      <c r="K41" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="L41" s="14">
-        <v>851</v>
-      </c>
-      <c r="M41" s="23">
+      <c r="L41" s="19">
         <f>E41/$E$7%</f>
         <v>29.347826086956523</v>
       </c>
-      <c r="N41" s="23">
-        <f t="shared" si="22"/>
+      <c r="M41" s="19">
+        <f t="shared" si="13"/>
         <v>20.017953321364452</v>
       </c>
-      <c r="O41" s="23">
-        <f t="shared" si="23"/>
+      <c r="N41" s="19">
+        <f t="shared" si="14"/>
         <v>14.958448753462605</v>
       </c>
-      <c r="P41" s="23">
+      <c r="O41" s="19">
         <f>H41/$H$7%</f>
         <v>9.418282548476455</v>
       </c>
-      <c r="T41" s="13" t="s">
+      <c r="Q41" s="12">
+        <v>851</v>
+      </c>
+      <c r="T41" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="U41" s="14">
+      <c r="U41" s="12">
         <v>851</v>
       </c>
-      <c r="V41" s="23">
+      <c r="V41" s="19">
         <f>E41/D41*100</f>
         <v>63.454759106933025</v>
       </c>
-      <c r="W41" s="23">
+      <c r="W41" s="19">
         <f>F41/D41*100</f>
         <v>26.204465334900117</v>
       </c>
-      <c r="X41" s="23">
+      <c r="X41" s="19">
         <f>G41/D41*100</f>
         <v>6.3454759106933016</v>
       </c>
-      <c r="Y41" s="23">
+      <c r="Y41" s="19">
         <f>H41/D41*100</f>
         <v>3.9952996474735603</v>
       </c>
-      <c r="Z41" s="24">
-        <f t="shared" si="15"/>
+      <c r="Z41" s="20">
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="2:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C42" s="13" t="s">
+    <row r="42" spans="2:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C42" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D42" s="21">
+      <c r="D42" s="17">
         <f>SUM(E42:H42)</f>
         <v>410</v>
       </c>
-      <c r="E42" s="14">
+      <c r="E42" s="12">
         <v>130</v>
       </c>
-      <c r="F42" s="14">
+      <c r="F42" s="12">
         <v>111</v>
       </c>
-      <c r="G42" s="14">
+      <c r="G42" s="12">
         <v>79</v>
       </c>
-      <c r="H42" s="14">
+      <c r="H42" s="12">
         <v>90</v>
       </c>
-      <c r="K42" s="13" t="s">
+      <c r="K42" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="L42" s="14">
+      <c r="L42" s="19">
+        <f t="shared" ref="L42" si="17">E42/$E$7%</f>
+        <v>7.0652173913043486</v>
+      </c>
+      <c r="M42" s="19">
+        <f t="shared" si="13"/>
+        <v>9.9640933572710946</v>
+      </c>
+      <c r="N42" s="19">
+        <f t="shared" si="14"/>
+        <v>21.883656509695292</v>
+      </c>
+      <c r="O42" s="19">
+        <f t="shared" ref="O42:O43" si="18">H42/$H$7%</f>
+        <v>24.930747922437675</v>
+      </c>
+      <c r="Q42" s="12">
         <v>410</v>
       </c>
-      <c r="M42" s="23">
-        <f t="shared" ref="M42" si="26">E42/$E$7%</f>
-        <v>7.0652173913043486</v>
-      </c>
-      <c r="N42" s="23">
-        <f t="shared" si="22"/>
-        <v>9.9640933572710946</v>
-      </c>
-      <c r="O42" s="23">
-        <f t="shared" si="23"/>
-        <v>21.883656509695292</v>
-      </c>
-      <c r="P42" s="23">
-        <f t="shared" ref="P42:P43" si="27">H42/$H$7%</f>
-        <v>24.930747922437675</v>
-      </c>
-      <c r="T42" s="13" t="s">
+      <c r="T42" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="U42" s="14">
+      <c r="U42" s="12">
         <v>410</v>
       </c>
-      <c r="V42" s="23">
+      <c r="V42" s="19">
         <f>E42/D42*100</f>
         <v>31.707317073170731</v>
       </c>
-      <c r="W42" s="23">
+      <c r="W42" s="19">
         <f>F42/D42*100</f>
         <v>27.073170731707318</v>
       </c>
-      <c r="X42" s="23">
+      <c r="X42" s="19">
         <f>G42/D42*100</f>
         <v>19.26829268292683</v>
       </c>
-      <c r="Y42" s="23">
+      <c r="Y42" s="19">
         <f>H42/D42*100</f>
         <v>21.951219512195124</v>
       </c>
-      <c r="Z42" s="24">
-        <f t="shared" si="15"/>
+      <c r="Z42" s="20">
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="2:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C43" s="13" t="s">
+    <row r="43" spans="2:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C43" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D43" s="21">
+      <c r="D43" s="17">
         <f>SUM(E43:H43)</f>
         <v>157</v>
       </c>
-      <c r="E43" s="14">
+      <c r="E43" s="12">
         <v>89</v>
       </c>
-      <c r="F43" s="14">
+      <c r="F43" s="12">
         <v>48</v>
       </c>
-      <c r="G43" s="14">
+      <c r="G43" s="12">
         <v>12</v>
       </c>
-      <c r="H43" s="14">
+      <c r="H43" s="12">
         <v>8</v>
       </c>
-      <c r="K43" s="13" t="s">
+      <c r="K43" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="L43" s="14">
-        <v>157</v>
-      </c>
-      <c r="M43" s="23">
+      <c r="L43" s="19">
         <f>E43/$E$7%</f>
         <v>4.8369565217391308</v>
       </c>
-      <c r="N43" s="23">
-        <f t="shared" si="22"/>
+      <c r="M43" s="19">
+        <f t="shared" si="13"/>
         <v>4.3087971274685817</v>
       </c>
-      <c r="O43" s="23">
-        <f t="shared" si="23"/>
+      <c r="N43" s="19">
+        <f t="shared" si="14"/>
         <v>3.32409972299169</v>
       </c>
-      <c r="P43" s="23">
-        <f t="shared" si="27"/>
+      <c r="O43" s="19">
+        <f t="shared" si="18"/>
         <v>2.21606648199446</v>
       </c>
-      <c r="T43" s="13" t="s">
+      <c r="Q43" s="12">
+        <v>157</v>
+      </c>
+      <c r="T43" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="U43" s="14">
+      <c r="U43" s="12">
         <v>157</v>
       </c>
-      <c r="V43" s="23">
+      <c r="V43" s="19">
         <f>E43/D43*100</f>
         <v>56.687898089171973</v>
       </c>
-      <c r="W43" s="23">
+      <c r="W43" s="19">
         <f>F43/D43*100</f>
         <v>30.573248407643312</v>
       </c>
-      <c r="X43" s="23">
+      <c r="X43" s="19">
         <f>G43/D43*100</f>
         <v>7.6433121019108281</v>
       </c>
-      <c r="Y43" s="23">
+      <c r="Y43" s="19">
         <f>H43/D43*100</f>
         <v>5.095541401273886</v>
       </c>
-      <c r="Z43" s="24">
-        <f t="shared" si="15"/>
+      <c r="Z43" s="20">
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
     </row>
-    <row r="44" spans="2:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="13" t="s">
+    <row r="44" spans="2:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D44" s="14"/>
-      <c r="E44" s="21">
+      <c r="D44" s="12"/>
+      <c r="E44" s="17">
         <f>SUM(E39:E43)</f>
         <v>2012</v>
       </c>
-      <c r="F44" s="21">
-        <f t="shared" ref="F44:H44" si="28">SUM(F39:F43)</f>
+      <c r="F44" s="17">
+        <f t="shared" ref="F44:H44" si="19">SUM(F39:F43)</f>
         <v>1246</v>
       </c>
-      <c r="G44" s="21">
-        <f t="shared" si="28"/>
+      <c r="G44" s="17">
+        <f t="shared" si="19"/>
         <v>387</v>
       </c>
-      <c r="H44" s="21">
-        <f t="shared" si="28"/>
+      <c r="H44" s="17">
+        <f t="shared" si="19"/>
         <v>393</v>
       </c>
-      <c r="J44" s="13" t="s">
+      <c r="J44" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="L44" s="14"/>
-      <c r="N44" s="23"/>
-      <c r="O44" s="23"/>
-      <c r="S44" s="13" t="s">
+      <c r="M44" s="19"/>
+      <c r="N44" s="19"/>
+      <c r="Q44" s="12"/>
+      <c r="S44" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="U44" s="14"/>
-      <c r="Z44" s="24">
-        <f t="shared" si="15"/>
+      <c r="U44" s="12"/>
+      <c r="Z44" s="20">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C45" s="13" t="s">
+    <row r="45" spans="2:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C45" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D45" s="21">
+      <c r="D45" s="17">
         <f>SUM(E45:H45)</f>
         <v>1638</v>
       </c>
-      <c r="E45" s="14">
+      <c r="E45" s="12">
         <v>909</v>
       </c>
-      <c r="F45" s="14">
+      <c r="F45" s="12">
         <v>496</v>
       </c>
-      <c r="G45" s="14">
+      <c r="G45" s="12">
         <v>115</v>
       </c>
-      <c r="H45" s="14">
+      <c r="H45" s="12">
         <v>118</v>
       </c>
-      <c r="K45" s="13" t="s">
+      <c r="K45" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L45" s="14">
-        <v>1638</v>
-      </c>
-      <c r="M45" s="23">
+      <c r="L45" s="19">
         <f>E45/$E$7%</f>
         <v>49.402173913043484</v>
       </c>
-      <c r="N45" s="23">
-        <f t="shared" ref="N45:N53" si="29">F45/$F$7%</f>
+      <c r="M45" s="19">
+        <f t="shared" ref="M45:M48" si="20">F45/$F$7%</f>
         <v>44.524236983842009</v>
       </c>
-      <c r="O45" s="23">
-        <f t="shared" ref="O45:O53" si="30">G45/$G$7%</f>
+      <c r="N45" s="19">
+        <f t="shared" ref="N45:N48" si="21">G45/$G$7%</f>
         <v>31.855955678670362</v>
       </c>
-      <c r="P45" s="23">
+      <c r="O45" s="19">
         <f>H45/$H$7%</f>
         <v>32.686980609418285</v>
       </c>
-      <c r="T45" s="13" t="s">
+      <c r="Q45" s="12">
+        <v>1638</v>
+      </c>
+      <c r="T45" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="U45" s="14">
+      <c r="U45" s="12">
         <v>1638</v>
       </c>
-      <c r="V45" s="23">
+      <c r="V45" s="19">
         <f>E45/D45*100</f>
         <v>55.494505494505496</v>
       </c>
-      <c r="W45" s="23">
+      <c r="W45" s="19">
         <f>F45/D45*100</f>
         <v>30.28083028083028</v>
       </c>
-      <c r="X45" s="23">
+      <c r="X45" s="19">
         <f>G45/D45*100</f>
         <v>7.0207570207570207</v>
       </c>
-      <c r="Y45" s="23">
+      <c r="Y45" s="19">
         <f>H45/D45*100</f>
         <v>7.2039072039072032</v>
       </c>
-      <c r="Z45" s="24">
-        <f t="shared" si="15"/>
+      <c r="Z45" s="20">
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="2:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C46" s="13" t="s">
+    <row r="46" spans="2:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C46" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D46" s="21">
+      <c r="D46" s="17">
         <f>SUM(E46:H46)</f>
         <v>760</v>
       </c>
-      <c r="E46" s="14">
+      <c r="E46" s="12">
         <v>393</v>
       </c>
-      <c r="F46" s="14">
+      <c r="F46" s="12">
         <v>223</v>
       </c>
-      <c r="G46" s="14">
+      <c r="G46" s="12">
         <v>80</v>
       </c>
-      <c r="H46" s="14">
+      <c r="H46" s="12">
         <v>64</v>
       </c>
-      <c r="K46" s="13" t="s">
+      <c r="K46" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="L46" s="14">
-        <v>760</v>
-      </c>
-      <c r="M46" s="23">
+      <c r="L46" s="19">
         <f>E46/$E$7%</f>
         <v>21.358695652173914</v>
       </c>
-      <c r="N46" s="23">
-        <f t="shared" si="29"/>
+      <c r="M46" s="19">
+        <f t="shared" si="20"/>
         <v>20.017953321364452</v>
       </c>
-      <c r="O46" s="23">
-        <f t="shared" si="30"/>
+      <c r="N46" s="19">
+        <f t="shared" si="21"/>
         <v>22.1606648199446</v>
       </c>
-      <c r="P46" s="23">
+      <c r="O46" s="19">
         <f>H46/$H$7%</f>
         <v>17.72853185595568</v>
       </c>
-      <c r="T46" s="13" t="s">
+      <c r="Q46" s="12">
+        <v>760</v>
+      </c>
+      <c r="T46" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="U46" s="14">
+      <c r="U46" s="12">
         <v>760</v>
       </c>
-      <c r="V46" s="23">
+      <c r="V46" s="19">
         <f>E46/D46*100</f>
         <v>51.710526315789473</v>
       </c>
-      <c r="W46" s="23">
+      <c r="W46" s="19">
         <f>F46/D46*100</f>
         <v>29.342105263157897</v>
       </c>
-      <c r="X46" s="23">
+      <c r="X46" s="19">
         <f>G46/D46*100</f>
         <v>10.526315789473683</v>
       </c>
-      <c r="Y46" s="23">
+      <c r="Y46" s="19">
         <f>H46/D46*100</f>
         <v>8.4210526315789469</v>
       </c>
-      <c r="Z46" s="24">
-        <f t="shared" si="15"/>
+      <c r="Z46" s="20">
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="2:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C47" s="13" t="s">
+    <row r="47" spans="2:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C47" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D47" s="21">
+      <c r="D47" s="17">
         <f>SUM(E47:H47)</f>
         <v>1279</v>
       </c>
-      <c r="E47" s="14">
+      <c r="E47" s="12">
         <v>538</v>
       </c>
-      <c r="F47" s="14">
+      <c r="F47" s="12">
         <v>395</v>
       </c>
-      <c r="G47" s="14">
+      <c r="G47" s="12">
         <v>161</v>
       </c>
-      <c r="H47" s="14">
+      <c r="H47" s="12">
         <v>185</v>
       </c>
-      <c r="K47" s="13" t="s">
+      <c r="K47" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="L47" s="14">
+      <c r="L47" s="19">
+        <f t="shared" ref="L47" si="22">E47/$E$7%</f>
+        <v>29.239130434782609</v>
+      </c>
+      <c r="M47" s="19">
+        <f t="shared" si="20"/>
+        <v>35.457809694793532</v>
+      </c>
+      <c r="N47" s="19">
+        <f t="shared" si="21"/>
+        <v>44.598337950138507</v>
+      </c>
+      <c r="O47" s="19">
+        <f t="shared" ref="O47:O48" si="23">H47/$H$7%</f>
+        <v>51.246537396121887</v>
+      </c>
+      <c r="Q47" s="12">
         <v>1279</v>
       </c>
-      <c r="M47" s="23">
-        <f t="shared" ref="M47" si="31">E47/$E$7%</f>
-        <v>29.239130434782609</v>
-      </c>
-      <c r="N47" s="23">
-        <f t="shared" si="29"/>
-        <v>35.457809694793532</v>
-      </c>
-      <c r="O47" s="23">
-        <f t="shared" si="30"/>
-        <v>44.598337950138507</v>
-      </c>
-      <c r="P47" s="23">
-        <f t="shared" ref="P47:P48" si="32">H47/$H$7%</f>
-        <v>51.246537396121887</v>
-      </c>
-      <c r="T47" s="13" t="s">
+      <c r="T47" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="U47" s="14">
+      <c r="U47" s="12">
         <v>1279</v>
       </c>
-      <c r="V47" s="23">
+      <c r="V47" s="19">
         <f>E47/D47*100</f>
         <v>42.064112587959343</v>
       </c>
-      <c r="W47" s="23">
+      <c r="W47" s="19">
         <f>F47/D47*100</f>
         <v>30.883502736512902</v>
       </c>
-      <c r="X47" s="23">
+      <c r="X47" s="19">
         <f>G47/D47*100</f>
         <v>12.587959343236903</v>
       </c>
-      <c r="Y47" s="23">
+      <c r="Y47" s="19">
         <f>H47/D47*100</f>
         <v>14.464425332290853</v>
       </c>
-      <c r="Z47" s="24">
-        <f t="shared" si="15"/>
+      <c r="Z47" s="20">
+        <f t="shared" si="6"/>
         <v>100.00000000000001</v>
       </c>
     </row>
-    <row r="48" spans="2:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C48" s="13" t="s">
+    <row r="48" spans="2:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C48" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D48" s="21">
+      <c r="D48" s="17">
         <f>SUM(E48:H48)</f>
         <v>361</v>
       </c>
-      <c r="E48" s="14">
+      <c r="E48" s="12">
         <v>172</v>
       </c>
-      <c r="F48" s="14">
+      <c r="F48" s="12">
         <v>132</v>
       </c>
-      <c r="G48" s="14">
+      <c r="G48" s="12">
         <v>31</v>
       </c>
-      <c r="H48" s="14">
+      <c r="H48" s="12">
         <v>26</v>
       </c>
-      <c r="K48" s="13" t="s">
+      <c r="K48" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="L48" s="14">
-        <v>361</v>
-      </c>
-      <c r="M48" s="23">
+      <c r="L48" s="19">
         <f>E48/$E$7%</f>
         <v>9.3478260869565233</v>
       </c>
-      <c r="N48" s="23">
-        <f t="shared" si="29"/>
+      <c r="M48" s="19">
+        <f t="shared" si="20"/>
         <v>11.849192100538598</v>
       </c>
-      <c r="O48" s="23">
-        <f t="shared" si="30"/>
+      <c r="N48" s="19">
+        <f t="shared" si="21"/>
         <v>8.5872576177285325</v>
       </c>
-      <c r="P48" s="23">
-        <f t="shared" si="32"/>
+      <c r="O48" s="19">
+        <f t="shared" si="23"/>
         <v>7.202216066481995</v>
       </c>
-      <c r="T48" s="13" t="s">
+      <c r="Q48" s="12">
+        <v>361</v>
+      </c>
+      <c r="T48" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="U48" s="14">
+      <c r="U48" s="12">
         <v>361</v>
       </c>
-      <c r="V48" s="23">
+      <c r="V48" s="19">
         <f>E48/D48*100</f>
         <v>47.64542936288089</v>
       </c>
-      <c r="W48" s="23">
+      <c r="W48" s="19">
         <f>F48/D48*100</f>
         <v>36.56509695290859</v>
       </c>
-      <c r="X48" s="23">
+      <c r="X48" s="19">
         <f>G48/D48*100</f>
         <v>8.5872576177285325</v>
       </c>
-      <c r="Y48" s="23">
+      <c r="Y48" s="19">
         <f>H48/D48*100</f>
         <v>7.202216066481995</v>
       </c>
-      <c r="Z48" s="24">
-        <f t="shared" si="15"/>
+      <c r="Z48" s="20">
+        <f t="shared" si="6"/>
         <v>100.00000000000001</v>
       </c>
     </row>
-    <row r="49" spans="2:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="13" t="s">
+    <row r="49" spans="2:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D49" s="14"/>
-      <c r="E49" s="21">
+      <c r="D49" s="12"/>
+      <c r="E49" s="17">
         <f>SUM(E45:E48)</f>
         <v>2012</v>
       </c>
-      <c r="F49" s="21">
-        <f t="shared" ref="F49:H49" si="33">SUM(F45:F48)</f>
+      <c r="F49" s="17">
+        <f t="shared" ref="F49:H49" si="24">SUM(F45:F48)</f>
         <v>1246</v>
       </c>
-      <c r="G49" s="21">
-        <f t="shared" si="33"/>
+      <c r="G49" s="17">
+        <f t="shared" si="24"/>
         <v>387</v>
       </c>
-      <c r="H49" s="21">
-        <f t="shared" si="33"/>
+      <c r="H49" s="17">
+        <f t="shared" si="24"/>
         <v>393</v>
       </c>
-      <c r="J49" s="13" t="s">
+      <c r="J49" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="L49" s="14"/>
-      <c r="N49" s="23"/>
-      <c r="O49" s="23"/>
-      <c r="S49" s="13" t="s">
+      <c r="M49" s="19"/>
+      <c r="N49" s="19"/>
+      <c r="Q49" s="12"/>
+      <c r="S49" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="U49" s="14"/>
-      <c r="Z49" s="24">
-        <f t="shared" si="15"/>
+      <c r="U49" s="12"/>
+      <c r="Z49" s="20">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C50" s="13" t="s">
+    <row r="50" spans="2:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C50" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D50" s="21">
-        <f t="shared" ref="D50:D51" si="34">SUM(E50:H50)</f>
+      <c r="D50" s="17">
+        <f t="shared" ref="D50:D51" si="25">SUM(E50:H50)</f>
         <v>815</v>
       </c>
-      <c r="E50" s="14">
+      <c r="E50" s="12">
         <v>451</v>
       </c>
-      <c r="F50" s="14">
+      <c r="F50" s="12">
         <v>258</v>
       </c>
-      <c r="G50" s="14">
+      <c r="G50" s="12">
         <v>53</v>
       </c>
-      <c r="H50" s="14">
+      <c r="H50" s="12">
         <v>53</v>
       </c>
-      <c r="K50" s="13" t="s">
+      <c r="K50" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="L50" s="14">
-        <v>815</v>
-      </c>
-      <c r="M50" s="23">
+      <c r="L50" s="19">
         <f>E50/$E$7%</f>
         <v>24.510869565217394</v>
       </c>
-      <c r="N50" s="23">
-        <f t="shared" ref="N50:N53" si="35">F50/$F$7%</f>
+      <c r="M50" s="19">
+        <f t="shared" ref="M50:M51" si="26">F50/$F$7%</f>
         <v>23.159784560143624</v>
       </c>
-      <c r="O50" s="23">
-        <f t="shared" ref="O50:O53" si="36">G50/$G$7%</f>
+      <c r="N50" s="19">
+        <f t="shared" ref="N50:N51" si="27">G50/$G$7%</f>
         <v>14.681440443213297</v>
       </c>
-      <c r="P50" s="23">
+      <c r="O50" s="19">
         <f>H50/$H$7%</f>
         <v>14.681440443213297</v>
       </c>
-      <c r="T50" s="13" t="s">
+      <c r="Q50" s="12">
+        <v>815</v>
+      </c>
+      <c r="T50" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="U50" s="14">
+      <c r="U50" s="12">
         <v>815</v>
       </c>
-      <c r="V50" s="23">
+      <c r="V50" s="19">
         <f>E50/D50*100</f>
         <v>55.337423312883438</v>
       </c>
-      <c r="W50" s="23">
+      <c r="W50" s="19">
         <f>F50/D50*100</f>
         <v>31.656441717791413</v>
       </c>
-      <c r="X50" s="23">
+      <c r="X50" s="19">
         <f>G50/D50*100</f>
         <v>6.5030674846625764</v>
       </c>
-      <c r="Y50" s="23">
+      <c r="Y50" s="19">
         <f>H50/D50*100</f>
         <v>6.5030674846625764</v>
       </c>
-      <c r="Z50" s="24">
-        <f t="shared" si="15"/>
+      <c r="Z50" s="20">
+        <f t="shared" si="6"/>
         <v>100.00000000000001</v>
       </c>
     </row>
-    <row r="51" spans="2:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C51" s="13" t="s">
+    <row r="51" spans="2:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C51" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D51" s="21">
-        <f t="shared" si="34"/>
+      <c r="D51" s="17">
+        <f t="shared" si="25"/>
         <v>2152</v>
       </c>
-      <c r="E51" s="14">
+      <c r="E51" s="12">
         <v>1172</v>
       </c>
-      <c r="F51" s="14">
+      <c r="F51" s="12">
         <v>644</v>
       </c>
-      <c r="G51" s="14">
+      <c r="G51" s="12">
         <v>177</v>
       </c>
-      <c r="H51" s="14">
+      <c r="H51" s="12">
         <v>159</v>
       </c>
-      <c r="K51" s="13" t="s">
+      <c r="K51" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="L51" s="14">
-        <v>2152</v>
-      </c>
-      <c r="M51" s="23">
+      <c r="L51" s="19">
         <f>E51/$E$7%</f>
         <v>63.695652173913047</v>
       </c>
-      <c r="N51" s="23">
-        <f t="shared" si="35"/>
+      <c r="M51" s="19">
+        <f t="shared" si="26"/>
         <v>57.809694793536799</v>
       </c>
-      <c r="O51" s="23">
-        <f t="shared" si="36"/>
+      <c r="N51" s="19">
+        <f t="shared" si="27"/>
         <v>49.030470914127427</v>
       </c>
-      <c r="P51" s="23">
-        <f t="shared" ref="P51" si="37">H51/$H$7%</f>
+      <c r="O51" s="19">
+        <f t="shared" ref="O51" si="28">H51/$H$7%</f>
         <v>44.044321329639892</v>
       </c>
-      <c r="S51" s="17"/>
-      <c r="T51" s="17" t="s">
+      <c r="Q51" s="12">
+        <v>2152</v>
+      </c>
+      <c r="S51" s="15"/>
+      <c r="T51" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="U51" s="18">
+      <c r="U51" s="16">
         <v>2152</v>
       </c>
-      <c r="V51" s="25">
+      <c r="V51" s="21">
         <f>E51/D51*100</f>
         <v>54.460966542750931</v>
       </c>
-      <c r="W51" s="25">
+      <c r="W51" s="21">
         <f>F51/D51*100</f>
         <v>29.92565055762082</v>
       </c>
-      <c r="X51" s="25">
+      <c r="X51" s="21">
         <f>G51/D51*100</f>
         <v>8.2249070631970262</v>
       </c>
-      <c r="Y51" s="25">
+      <c r="Y51" s="21">
         <f>H51/D51*100</f>
         <v>7.3884758364312271</v>
       </c>
-      <c r="Z51" s="24">
-        <f t="shared" si="15"/>
+      <c r="Z51" s="20">
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="2:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C52" s="13" t="s">
+    <row r="52" spans="2:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C52" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D52" s="21">
+      <c r="D52" s="17">
         <f>SUM(E52:H52)</f>
         <v>1071</v>
       </c>
-      <c r="E52" s="14">
+      <c r="E52" s="12">
         <v>389</v>
       </c>
-      <c r="F52" s="14">
+      <c r="F52" s="12">
         <v>344</v>
       </c>
-      <c r="G52" s="14">
+      <c r="G52" s="12">
         <v>157</v>
       </c>
-      <c r="H52" s="14">
+      <c r="H52" s="12">
         <v>181</v>
       </c>
-      <c r="J52" s="17"/>
-      <c r="K52" s="17" t="s">
+      <c r="J52" s="15"/>
+      <c r="K52" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="L52" s="18">
-        <v>1071</v>
-      </c>
-      <c r="M52" s="25">
+      <c r="L52" s="21">
         <f>E52/$E$7%</f>
         <v>21.14130434782609</v>
       </c>
-      <c r="N52" s="25">
+      <c r="M52" s="21">
         <f>F52/$F$7%</f>
         <v>30.879712746858168</v>
       </c>
-      <c r="O52" s="25">
+      <c r="N52" s="21">
         <f>G52/$G$7%</f>
         <v>43.490304709141277</v>
       </c>
-      <c r="P52" s="25">
+      <c r="O52" s="21">
         <f>H52/$H$7%</f>
         <v>50.138504155124657</v>
       </c>
-      <c r="Q52" s="17"/>
-      <c r="T52" s="13" t="s">
+      <c r="P52" s="15"/>
+      <c r="Q52" s="16">
+        <v>1071</v>
+      </c>
+      <c r="T52" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="U52" s="14">
+      <c r="U52" s="12">
         <v>1071</v>
       </c>
-      <c r="V52" s="23">
+      <c r="V52" s="19">
         <f>E52/D52*100</f>
         <v>36.321195144724555</v>
       </c>
-      <c r="W52" s="23">
+      <c r="W52" s="19">
         <f>F52/D52*100</f>
         <v>32.119514472455649</v>
       </c>
-      <c r="X52" s="23">
+      <c r="X52" s="19">
         <f>G52/D52*100</f>
         <v>14.65919701213819</v>
       </c>
-      <c r="Y52" s="23">
+      <c r="Y52" s="19">
         <f>H52/D52*100</f>
         <v>16.900093370681606</v>
       </c>
-      <c r="Z52" s="24">
+      <c r="Z52" s="20">
         <f>SUM(V52:Y52)</f>
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="2:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D53" s="14"/>
-      <c r="E53" s="21">
+    <row r="53" spans="2:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D53" s="12"/>
+      <c r="E53" s="17">
         <f>SUM(E50:E52)</f>
         <v>2012</v>
       </c>
-      <c r="F53" s="21">
-        <f t="shared" ref="F53:H53" si="38">SUM(F50:F52)</f>
+      <c r="F53" s="17">
+        <f t="shared" ref="F53:H53" si="29">SUM(F50:F52)</f>
         <v>1246</v>
       </c>
-      <c r="G53" s="21">
-        <f t="shared" si="38"/>
+      <c r="G53" s="17">
+        <f t="shared" si="29"/>
         <v>387</v>
       </c>
-      <c r="H53" s="21">
-        <f t="shared" si="38"/>
+      <c r="H53" s="17">
+        <f t="shared" si="29"/>
         <v>393</v>
       </c>
-      <c r="U53" s="14"/>
+      <c r="U53" s="12"/>
     </row>
     <row r="57" spans="2:26" x14ac:dyDescent="0.25">
       <c r="C57">
@@ -3548,8 +3560,8 @@
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="V4:Y4"/>
-    <mergeCell ref="M3:P3"/>
-    <mergeCell ref="M31:P31"/>
+    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="L31:O31"/>
     <mergeCell ref="V31:Y31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3557,7 +3569,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{77EDBE04-127B-4D30-9AC8-FAA1BDCAF585}">
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{0A184D5A-B882-4B3C-A16A-BC2831429DCD}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -3568,88 +3580,176 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Sheet1!M32:P32</xm:f>
-              <xm:sqref>Q32</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M33:P33</xm:f>
-              <xm:sqref>Q33</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M34:P34</xm:f>
-              <xm:sqref>Q34</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M35:P35</xm:f>
-              <xm:sqref>Q35</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M36:P36</xm:f>
-              <xm:sqref>Q36</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M37:P37</xm:f>
-              <xm:sqref>Q37</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M38:P38</xm:f>
-              <xm:sqref>Q38</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M39:P39</xm:f>
-              <xm:sqref>Q39</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M40:P40</xm:f>
-              <xm:sqref>Q40</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M41:P41</xm:f>
-              <xm:sqref>Q41</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M42:P42</xm:f>
-              <xm:sqref>Q42</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M43:P43</xm:f>
-              <xm:sqref>Q43</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M44:P44</xm:f>
-              <xm:sqref>Q44</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M45:P45</xm:f>
-              <xm:sqref>Q45</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M46:P46</xm:f>
-              <xm:sqref>Q46</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M47:P47</xm:f>
-              <xm:sqref>Q47</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M48:P48</xm:f>
-              <xm:sqref>Q48</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M49:P49</xm:f>
-              <xm:sqref>Q49</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M50:P50</xm:f>
-              <xm:sqref>Q50</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M51:P51</xm:f>
-              <xm:sqref>Q51</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M52:P52</xm:f>
-              <xm:sqref>Q52</xm:sqref>
+              <xm:f>Sheet1!L5:O5</xm:f>
+              <xm:sqref>P5</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L6:O6</xm:f>
+              <xm:sqref>P6</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L7:O7</xm:f>
+              <xm:sqref>P7</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L8:O8</xm:f>
+              <xm:sqref>P8</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L9:O9</xm:f>
+              <xm:sqref>P9</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L10:O10</xm:f>
+              <xm:sqref>P10</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L11:O11</xm:f>
+              <xm:sqref>P11</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L12:O12</xm:f>
+              <xm:sqref>P12</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L13:O13</xm:f>
+              <xm:sqref>P13</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L14:O14</xm:f>
+              <xm:sqref>P14</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L15:O15</xm:f>
+              <xm:sqref>P15</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L16:O16</xm:f>
+              <xm:sqref>P16</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L17:O17</xm:f>
+              <xm:sqref>P17</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L18:O18</xm:f>
+              <xm:sqref>P18</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L19:O19</xm:f>
+              <xm:sqref>P19</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L20:O20</xm:f>
+              <xm:sqref>P20</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L21:O21</xm:f>
+              <xm:sqref>P21</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L22:O22</xm:f>
+              <xm:sqref>P22</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L23:O23</xm:f>
+              <xm:sqref>P23</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L24:O24</xm:f>
+              <xm:sqref>P24</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{9309082F-C68D-4BE0-B6FB-5BBCC7127EC3}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Sheet1!V5:Y5</xm:f>
+              <xm:sqref>AA5</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!V6:Y6</xm:f>
+              <xm:sqref>AA6</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!V7:Y7</xm:f>
+              <xm:sqref>AA7</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!V8:Y8</xm:f>
+              <xm:sqref>AA8</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!V9:Y9</xm:f>
+              <xm:sqref>AA9</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!V10:Y10</xm:f>
+              <xm:sqref>AA10</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!V11:Y11</xm:f>
+              <xm:sqref>AA11</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!V12:Y12</xm:f>
+              <xm:sqref>AA12</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!V13:Y13</xm:f>
+              <xm:sqref>AA13</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!V14:Y14</xm:f>
+              <xm:sqref>AA14</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!V15:Y15</xm:f>
+              <xm:sqref>AA15</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!V16:Y16</xm:f>
+              <xm:sqref>AA16</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!V17:Y17</xm:f>
+              <xm:sqref>AA17</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!V18:Y18</xm:f>
+              <xm:sqref>AA18</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!V19:Y19</xm:f>
+              <xm:sqref>AA19</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!V20:Y20</xm:f>
+              <xm:sqref>AA20</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!V21:Y21</xm:f>
+              <xm:sqref>AA21</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!V22:Y22</xm:f>
+              <xm:sqref>AA22</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!V23:Y23</xm:f>
+              <xm:sqref>AA23</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!V24:Y24</xm:f>
+              <xm:sqref>AA24</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -3749,7 +3849,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{9309082F-C68D-4BE0-B6FB-5BBCC7127EC3}">
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{77EDBE04-127B-4D30-9AC8-FAA1BDCAF585}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -3760,176 +3860,88 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Sheet1!V5:Y5</xm:f>
-              <xm:sqref>AA5</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!V6:Y6</xm:f>
-              <xm:sqref>AA6</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!V7:Y7</xm:f>
-              <xm:sqref>AA7</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!V8:Y8</xm:f>
-              <xm:sqref>AA8</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!V9:Y9</xm:f>
-              <xm:sqref>AA9</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!V10:Y10</xm:f>
-              <xm:sqref>AA10</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!V11:Y11</xm:f>
-              <xm:sqref>AA11</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!V12:Y12</xm:f>
-              <xm:sqref>AA12</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!V13:Y13</xm:f>
-              <xm:sqref>AA13</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!V14:Y14</xm:f>
-              <xm:sqref>AA14</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!V15:Y15</xm:f>
-              <xm:sqref>AA15</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!V16:Y16</xm:f>
-              <xm:sqref>AA16</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!V17:Y17</xm:f>
-              <xm:sqref>AA17</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!V18:Y18</xm:f>
-              <xm:sqref>AA18</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!V19:Y19</xm:f>
-              <xm:sqref>AA19</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!V20:Y20</xm:f>
-              <xm:sqref>AA20</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!V21:Y21</xm:f>
-              <xm:sqref>AA21</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!V22:Y22</xm:f>
-              <xm:sqref>AA22</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!V23:Y23</xm:f>
-              <xm:sqref>AA23</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!V24:Y24</xm:f>
-              <xm:sqref>AA24</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{0A184D5A-B882-4B3C-A16A-BC2831429DCD}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>Sheet1!M5:P5</xm:f>
-              <xm:sqref>Q5</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M6:P6</xm:f>
-              <xm:sqref>Q6</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M7:P7</xm:f>
-              <xm:sqref>Q7</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M8:P8</xm:f>
-              <xm:sqref>Q8</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M9:P9</xm:f>
-              <xm:sqref>Q9</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M10:P10</xm:f>
-              <xm:sqref>Q10</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M11:P11</xm:f>
-              <xm:sqref>Q11</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M12:P12</xm:f>
-              <xm:sqref>Q12</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M13:P13</xm:f>
-              <xm:sqref>Q13</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M14:P14</xm:f>
-              <xm:sqref>Q14</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M15:P15</xm:f>
-              <xm:sqref>Q15</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M16:P16</xm:f>
-              <xm:sqref>Q16</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M17:P17</xm:f>
-              <xm:sqref>Q17</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M18:P18</xm:f>
-              <xm:sqref>Q18</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M19:P19</xm:f>
-              <xm:sqref>Q19</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M20:P20</xm:f>
-              <xm:sqref>Q20</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M21:P21</xm:f>
-              <xm:sqref>Q21</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M22:P22</xm:f>
-              <xm:sqref>Q22</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M23:P23</xm:f>
-              <xm:sqref>Q23</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M24:P24</xm:f>
-              <xm:sqref>Q24</xm:sqref>
+              <xm:f>Sheet1!L32:O32</xm:f>
+              <xm:sqref>P32</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L33:O33</xm:f>
+              <xm:sqref>P33</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L34:O34</xm:f>
+              <xm:sqref>P34</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L35:O35</xm:f>
+              <xm:sqref>P35</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L36:O36</xm:f>
+              <xm:sqref>P36</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L37:O37</xm:f>
+              <xm:sqref>P37</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L38:O38</xm:f>
+              <xm:sqref>P38</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L39:O39</xm:f>
+              <xm:sqref>P39</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L40:O40</xm:f>
+              <xm:sqref>P40</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L41:O41</xm:f>
+              <xm:sqref>P41</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L42:O42</xm:f>
+              <xm:sqref>P42</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L43:O43</xm:f>
+              <xm:sqref>P43</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L44:O44</xm:f>
+              <xm:sqref>P44</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L45:O45</xm:f>
+              <xm:sqref>P45</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L46:O46</xm:f>
+              <xm:sqref>P46</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L47:O47</xm:f>
+              <xm:sqref>P47</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L48:O48</xm:f>
+              <xm:sqref>P48</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L49:O49</xm:f>
+              <xm:sqref>P49</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L50:O50</xm:f>
+              <xm:sqref>P50</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L51:O51</xm:f>
+              <xm:sqref>P51</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!L52:O52</xm:f>
+              <xm:sqref>P52</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>

</xml_diff>

<commit_message>
number of 4xx products
</commit_message>
<xml_diff>
--- a/eg_data/NHANES/PF/Waist2/Demog/Demog.xlsx
+++ b/eg_data/NHANES/PF/Waist2/Demog/Demog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadoh\OneDrive\Documents\GitHub\DietR\eg_data\NHANES\PF\Waist2\Demog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3989D3AA-A14F-4C34-A55C-4C0294C8DC19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544122C8-34CA-4B85-BB12-7BE36854F817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26010" yWindow="-2880" windowWidth="21510" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20145" yWindow="-2970" windowWidth="28275" windowHeight="14430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
     <author>tc={6B71FC00-6E35-43E5-AA19-CBFB515381FE}</author>
   </authors>
   <commentList>
-    <comment ref="S2" authorId="0" shapeId="0" xr:uid="{2C5AD34B-0D2F-464C-8814-9F000872949B}">
+    <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{2C5AD34B-0D2F-464C-8814-9F000872949B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="36">
   <si>
     <t>Gender</t>
   </si>
@@ -167,14 +167,20 @@
     <t>p-difference</t>
   </si>
   <si>
-    <t>p-trend</t>
+    <t>p-Chi sq.</t>
+  </si>
+  <si>
+    <t>&lt; 0.0001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,12 +201,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -268,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -323,6 +323,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -335,20 +337,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -637,7 +628,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="S2" dT="2023-05-26T04:52:50.62" personId="{0428676E-8216-4833-A51F-E760E10D3DEE}" id="{2C5AD34B-0D2F-464C-8814-9F000872949B}">
+  <threadedComment ref="Q2" dT="2023-05-26T04:52:50.62" personId="{0428676E-8216-4833-A51F-E760E10D3DEE}" id="{2C5AD34B-0D2F-464C-8814-9F000872949B}">
     <text>Tests whether the demographic categories (column K) and DivGroups are independent or not.</text>
   </threadedComment>
   <threadedComment ref="I3" dT="2023-05-26T04:52:50.62" personId="{0428676E-8216-4833-A51F-E760E10D3DEE}" id="{6B71FC00-6E35-43E5-AA19-CBFB515381FE}">
@@ -651,7 +642,7 @@
   <dimension ref="B1:AB68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,18 +673,16 @@
       <c r="P1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="Q1" s="1"/>
+      <c r="S1" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="S1" s="28" t="s">
-        <v>32</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="M2" s="1" t="str">
@@ -731,15 +720,17 @@
       </c>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
-      <c r="M3" s="24" t="s">
+      <c r="M3" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="4"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="32" t="s">
+        <v>34</v>
+      </c>
       <c r="R3" s="4"/>
-      <c r="S3" s="29"/>
+      <c r="S3" s="4"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
       <c r="W3" s="3" t="s">
@@ -759,10 +750,10 @@
       </c>
     </row>
     <row r="4" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="31"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
         <v>28</v>
@@ -776,27 +767,27 @@
       <c r="H4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="31">
+      <c r="I4" s="30">
         <v>8.4180000000000005E-2</v>
       </c>
       <c r="K4" t="s">
         <v>0</v>
       </c>
-      <c r="R4" s="1"/>
-      <c r="S4" s="35" t="s">
-        <v>34</v>
-      </c>
+      <c r="Q4" s="1">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="S4" s="1"/>
       <c r="U4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="V4" s="4"/>
       <c r="W4" s="5"/>
-      <c r="X4" s="24" t="s">
+      <c r="X4" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="Y4" s="25"/>
-      <c r="Z4" s="25"/>
-      <c r="AA4" s="25"/>
+      <c r="Y4" s="27"/>
+      <c r="Z4" s="27"/>
+      <c r="AA4" s="27"/>
     </row>
     <row r="5" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
@@ -818,6 +809,7 @@
       <c r="H5" s="1">
         <v>172</v>
       </c>
+      <c r="I5" s="31"/>
       <c r="L5" t="s">
         <v>1</v>
       </c>
@@ -837,11 +829,11 @@
         <f>H5/$H$8%</f>
         <v>47.64542936288089</v>
       </c>
-      <c r="R5" s="1">
+      <c r="Q5" s="1"/>
+      <c r="S5" s="1">
         <f>IFERROR(D5,"")</f>
         <v>1745</v>
       </c>
-      <c r="S5" s="1"/>
       <c r="U5" s="2"/>
       <c r="V5" s="2" t="s">
         <v>1</v>
@@ -890,6 +882,7 @@
       <c r="H6" s="1">
         <v>189</v>
       </c>
+      <c r="I6" s="31"/>
       <c r="L6" t="s">
         <v>2</v>
       </c>
@@ -909,11 +902,11 @@
         <f>H6/$H$8%</f>
         <v>52.354570637119117</v>
       </c>
-      <c r="R6" s="1">
+      <c r="Q6" s="1"/>
+      <c r="S6" s="1">
         <f>IFERROR(D6,"")</f>
         <v>1931</v>
       </c>
-      <c r="S6" s="1"/>
       <c r="V6" t="s">
         <v>2</v>
       </c>
@@ -947,14 +940,15 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="L7" s="33" t="s">
+      <c r="I7" s="31"/>
+      <c r="L7" s="25" t="s">
         <v>33</v>
       </c>
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
-      <c r="R7" s="1"/>
+      <c r="Q7" s="1"/>
       <c r="S7" s="1"/>
       <c r="X7" s="7"/>
       <c r="Y7" s="7"/>
@@ -963,7 +957,7 @@
       <c r="AB7" s="9"/>
     </row>
     <row r="8" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="24" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="1"/>
@@ -983,14 +977,16 @@
         <f t="shared" si="1"/>
         <v>361</v>
       </c>
-      <c r="I8" s="31">
+      <c r="I8" s="30">
         <v>8.2019999999999992E-3</v>
       </c>
       <c r="K8" t="s">
         <v>13</v>
       </c>
       <c r="N8" s="7"/>
-      <c r="R8" s="1"/>
+      <c r="Q8" s="1">
+        <v>8.0000000000000002E-3</v>
+      </c>
       <c r="S8" s="1"/>
       <c r="U8" t="s">
         <v>13</v>
@@ -1020,6 +1016,7 @@
       <c r="H9" s="1">
         <v>122</v>
       </c>
+      <c r="I9" s="31"/>
       <c r="L9" t="s">
         <v>22</v>
       </c>
@@ -1039,11 +1036,11 @@
         <f>H9/$H$8%</f>
         <v>33.795013850415515</v>
       </c>
-      <c r="R9" s="1">
+      <c r="Q9" s="1"/>
+      <c r="S9" s="1">
         <f>IFERROR(D9,"")</f>
         <v>1320</v>
       </c>
-      <c r="S9" s="1"/>
       <c r="V9" t="s">
         <v>22</v>
       </c>
@@ -1091,6 +1088,7 @@
       <c r="H10" s="1">
         <v>119</v>
       </c>
+      <c r="I10" s="31"/>
       <c r="L10" t="s">
         <v>23</v>
       </c>
@@ -1110,11 +1108,11 @@
         <f>H10/$H$8%</f>
         <v>32.963988919667592</v>
       </c>
-      <c r="R10" s="1">
+      <c r="Q10" s="1"/>
+      <c r="S10" s="1">
         <f>IFERROR(D10,"")</f>
         <v>1190</v>
       </c>
-      <c r="S10" s="1"/>
       <c r="V10" t="s">
         <v>23</v>
       </c>
@@ -1162,6 +1160,7 @@
       <c r="H11" s="1">
         <v>120</v>
       </c>
+      <c r="I11" s="31"/>
       <c r="L11" t="s">
         <v>24</v>
       </c>
@@ -1181,11 +1180,11 @@
         <f>H11/$H$8%</f>
         <v>33.2409972299169</v>
       </c>
-      <c r="R11" s="1">
+      <c r="Q11" s="1"/>
+      <c r="S11" s="1">
         <f>IFERROR(D11,"")</f>
         <v>1166</v>
       </c>
-      <c r="S11" s="1"/>
       <c r="V11" t="s">
         <v>24</v>
       </c>
@@ -1219,14 +1218,13 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="L12" s="33" t="s">
-        <v>34</v>
-      </c>
+      <c r="I12" s="31"/>
+      <c r="L12" s="25"/>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
       <c r="P12" s="7"/>
-      <c r="R12" s="1"/>
+      <c r="Q12" s="1"/>
       <c r="S12" s="1"/>
       <c r="X12" s="7"/>
       <c r="Y12" s="7"/>
@@ -1235,7 +1233,7 @@
       <c r="AB12" s="9"/>
     </row>
     <row r="13" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="24" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="1"/>
@@ -1255,7 +1253,7 @@
         <f t="shared" si="2"/>
         <v>361</v>
       </c>
-      <c r="I13" s="32">
+      <c r="I13" s="30">
         <v>2.2E-16</v>
       </c>
       <c r="K13" t="s">
@@ -1263,7 +1261,9 @@
       </c>
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
-      <c r="R13" s="1"/>
+      <c r="Q13" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S13" s="1"/>
       <c r="U13" t="s">
         <v>3</v>
@@ -1293,6 +1293,7 @@
       <c r="H14" s="1">
         <v>117</v>
       </c>
+      <c r="I14" s="31"/>
       <c r="L14" t="s">
         <v>25</v>
       </c>
@@ -1312,11 +1313,11 @@
         <f>H14/$H$8%</f>
         <v>32.409972299168977</v>
       </c>
-      <c r="R14" s="1">
+      <c r="Q14" s="1"/>
+      <c r="S14" s="1">
         <f>IFERROR(D14,"")</f>
         <v>1092</v>
       </c>
-      <c r="S14" s="1"/>
       <c r="V14" t="s">
         <v>25</v>
       </c>
@@ -1364,6 +1365,7 @@
       <c r="H15" s="1">
         <v>130</v>
       </c>
+      <c r="I15" s="31"/>
       <c r="L15" t="s">
         <v>4</v>
       </c>
@@ -1383,11 +1385,11 @@
         <f>H15/$H$8%</f>
         <v>36.011080332409975</v>
       </c>
-      <c r="R15" s="1">
+      <c r="Q15" s="1"/>
+      <c r="S15" s="1">
         <f>IFERROR(D15,"")</f>
         <v>1328</v>
       </c>
-      <c r="S15" s="1"/>
       <c r="V15" t="s">
         <v>4</v>
       </c>
@@ -1435,6 +1437,7 @@
       <c r="H16" s="1">
         <v>34</v>
       </c>
+      <c r="I16" s="31"/>
       <c r="L16" t="s">
         <v>5</v>
       </c>
@@ -1454,11 +1457,11 @@
         <f>H16/$H$8%</f>
         <v>9.418282548476455</v>
       </c>
-      <c r="R16" s="1">
+      <c r="Q16" s="1"/>
+      <c r="S16" s="1">
         <f>IFERROR(D16,"")</f>
         <v>753</v>
       </c>
-      <c r="S16" s="1"/>
       <c r="V16" t="s">
         <v>5</v>
       </c>
@@ -1506,6 +1509,7 @@
       <c r="H17" s="1">
         <v>74</v>
       </c>
+      <c r="I17" s="31"/>
       <c r="L17" t="s">
         <v>6</v>
       </c>
@@ -1525,11 +1529,11 @@
         <f>H17/$H$8%</f>
         <v>20.498614958448755</v>
       </c>
-      <c r="R17" s="1">
+      <c r="Q17" s="1"/>
+      <c r="S17" s="1">
         <f>IFERROR(D17,"")</f>
         <v>363</v>
       </c>
-      <c r="S17" s="1"/>
       <c r="V17" t="s">
         <v>6</v>
       </c>
@@ -1577,6 +1581,7 @@
       <c r="H18" s="1">
         <v>6</v>
       </c>
+      <c r="I18" s="31"/>
       <c r="L18" t="s">
         <v>14</v>
       </c>
@@ -1596,11 +1601,11 @@
         <f>H18/$H$8%</f>
         <v>1.662049861495845</v>
       </c>
-      <c r="R18" s="1">
+      <c r="Q18" s="1"/>
+      <c r="S18" s="1">
         <f>IFERROR(D18,"")</f>
         <v>140</v>
       </c>
-      <c r="S18" s="1"/>
       <c r="V18" t="s">
         <v>14</v>
       </c>
@@ -1634,14 +1639,13 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="L19" s="33" t="s">
-        <v>33</v>
-      </c>
+      <c r="I19" s="31"/>
+      <c r="L19" s="25"/>
       <c r="M19" s="7"/>
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
       <c r="P19" s="7"/>
-      <c r="R19" s="1"/>
+      <c r="Q19" s="1"/>
       <c r="S19" s="1"/>
       <c r="X19" s="7"/>
       <c r="Y19" s="7"/>
@@ -1650,7 +1654,7 @@
       <c r="AB19" s="9"/>
     </row>
     <row r="20" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="24" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="1"/>
@@ -1670,7 +1674,7 @@
         <f t="shared" si="3"/>
         <v>361</v>
       </c>
-      <c r="I20" s="32">
+      <c r="I20" s="30">
         <v>2.2E-16</v>
       </c>
       <c r="K20" t="s">
@@ -1678,7 +1682,9 @@
       </c>
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
-      <c r="R20" s="1"/>
+      <c r="Q20" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S20" s="1"/>
       <c r="U20" t="s">
         <v>7</v>
@@ -1708,6 +1714,7 @@
       <c r="H21" s="1">
         <v>124</v>
       </c>
+      <c r="I21" s="31"/>
       <c r="L21" t="s">
         <v>15</v>
       </c>
@@ -1727,11 +1734,11 @@
         <f>H21/$H$8%</f>
         <v>34.34903047091413</v>
       </c>
-      <c r="R21" s="1">
+      <c r="Q21" s="1"/>
+      <c r="S21" s="1">
         <f>IFERROR(D21,"")</f>
         <v>1638</v>
       </c>
-      <c r="S21" s="1"/>
       <c r="V21" t="s">
         <v>15</v>
       </c>
@@ -1779,6 +1786,7 @@
       <c r="H22" s="1">
         <v>60</v>
       </c>
+      <c r="I22" s="31"/>
       <c r="L22" t="s">
         <v>17</v>
       </c>
@@ -1798,11 +1806,11 @@
         <f>H22/$H$8%</f>
         <v>16.62049861495845</v>
       </c>
-      <c r="R22" s="1">
+      <c r="Q22" s="1"/>
+      <c r="S22" s="1">
         <f>IFERROR(D22,"")</f>
         <v>760</v>
       </c>
-      <c r="S22" s="1"/>
       <c r="V22" t="s">
         <v>17</v>
       </c>
@@ -1850,6 +1858,7 @@
       <c r="H23" s="1">
         <v>177</v>
       </c>
+      <c r="I23" s="31"/>
       <c r="L23" t="s">
         <v>16</v>
       </c>
@@ -1869,11 +1878,11 @@
         <f>H23/$H$8%</f>
         <v>49.030470914127427</v>
       </c>
-      <c r="R23" s="1">
+      <c r="Q23" s="1"/>
+      <c r="S23" s="1">
         <f>IFERROR(D23,"")</f>
         <v>1278</v>
       </c>
-      <c r="S23" s="1"/>
       <c r="V23" t="s">
         <v>16</v>
       </c>
@@ -1907,14 +1916,13 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-      <c r="L24" s="33" t="s">
-        <v>34</v>
-      </c>
+      <c r="I24" s="31"/>
+      <c r="L24" s="25"/>
       <c r="M24" s="7"/>
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
       <c r="P24" s="7"/>
-      <c r="R24" s="1"/>
+      <c r="Q24" s="1"/>
       <c r="S24" s="1"/>
       <c r="X24" s="7"/>
       <c r="Y24" s="7"/>
@@ -1923,7 +1931,7 @@
       <c r="AB24" s="9"/>
     </row>
     <row r="25" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="24" t="s">
         <v>8</v>
       </c>
       <c r="D25" s="1"/>
@@ -1943,7 +1951,7 @@
         <f>SUM(H21:H23)</f>
         <v>361</v>
       </c>
-      <c r="I25" s="32">
+      <c r="I25" s="30">
         <v>2.2E-16</v>
       </c>
       <c r="K25" t="s">
@@ -1951,7 +1959,9 @@
       </c>
       <c r="N25" s="7"/>
       <c r="O25" s="7"/>
-      <c r="R25" s="1"/>
+      <c r="Q25" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="S25" s="1"/>
       <c r="U25" t="s">
         <v>8</v>
@@ -1981,6 +1991,7 @@
       <c r="H26" s="1">
         <v>51</v>
       </c>
+      <c r="I26" s="31"/>
       <c r="L26" t="s">
         <v>19</v>
       </c>
@@ -2000,11 +2011,11 @@
         <f>H26/$H$8%</f>
         <v>14.127423822714682</v>
       </c>
-      <c r="R26" s="1">
+      <c r="Q26" s="1"/>
+      <c r="S26" s="1">
         <f>IFERROR(D26,"")</f>
         <v>720</v>
       </c>
-      <c r="S26" s="1"/>
       <c r="V26" t="s">
         <v>19</v>
       </c>
@@ -2052,6 +2063,7 @@
       <c r="H27" s="1">
         <v>152</v>
       </c>
+      <c r="I27" s="31"/>
       <c r="L27" t="s">
         <v>21</v>
       </c>
@@ -2071,11 +2083,11 @@
         <f>H27/$H$8%</f>
         <v>42.10526315789474</v>
       </c>
-      <c r="R27" s="1">
+      <c r="Q27" s="1"/>
+      <c r="S27" s="1">
         <f>IFERROR(D27,"")</f>
         <v>1965</v>
       </c>
-      <c r="S27" s="1"/>
       <c r="U27" s="4"/>
       <c r="V27" s="4" t="s">
         <v>21</v>
@@ -2124,32 +2136,31 @@
       <c r="H28" s="1">
         <v>158</v>
       </c>
-      <c r="K28" s="29"/>
-      <c r="L28" s="29" t="s">
+      <c r="I28" s="31"/>
+      <c r="L28" t="s">
         <v>20</v>
       </c>
-      <c r="M28" s="34">
+      <c r="M28" s="7">
         <f>E28/$E$8%</f>
         <v>19.728260869565219</v>
       </c>
-      <c r="N28" s="34">
+      <c r="N28" s="7">
         <f>F28/$F$8%</f>
         <v>28.00718132854578</v>
       </c>
-      <c r="O28" s="34">
+      <c r="O28" s="7">
         <f>G28/$G$8%</f>
         <v>43.767313019390585</v>
       </c>
-      <c r="P28" s="34">
+      <c r="P28" s="7">
         <f>H28/$H$8%</f>
         <v>43.767313019390585</v>
       </c>
-      <c r="Q28" s="29"/>
-      <c r="R28" s="28">
+      <c r="Q28" s="1"/>
+      <c r="S28" s="1">
         <f>IFERROR(D28,"")</f>
         <v>991</v>
       </c>
-      <c r="S28" s="28"/>
       <c r="V28" t="s">
         <v>20</v>
       </c>
@@ -2181,17 +2192,14 @@
       <c r="D29" s="10"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
-      <c r="K29" s="29"/>
-      <c r="L29" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="M29" s="34"/>
-      <c r="N29" s="34"/>
-      <c r="O29" s="34"/>
-      <c r="P29" s="34"/>
-      <c r="Q29" s="29"/>
-      <c r="R29" s="28"/>
-      <c r="S29" s="28"/>
+      <c r="I29" s="31"/>
+      <c r="L29" s="25"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="1"/>
+      <c r="S29" s="1"/>
       <c r="X29" s="7"/>
       <c r="Y29" s="7"/>
       <c r="Z29" s="7"/>
@@ -2216,6 +2224,7 @@
         <f t="shared" si="5"/>
         <v>361</v>
       </c>
+      <c r="I30" s="31"/>
     </row>
     <row r="31" spans="2:28" x14ac:dyDescent="0.25">
       <c r="D31" s="1"/>
@@ -2223,6 +2232,7 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
+      <c r="I31" s="31"/>
       <c r="M31" s="9"/>
       <c r="N31" s="9"/>
       <c r="O31" s="9"/>
@@ -2278,10 +2288,10 @@
       <c r="P35" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="R35" s="14" t="s">
+      <c r="Q35" s="12"/>
+      <c r="S35" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="S35" s="30"/>
       <c r="U35" s="13"/>
       <c r="V35" s="13"/>
       <c r="W35" s="14" t="s">
@@ -2321,25 +2331,25 @@
         <v>0</v>
       </c>
       <c r="L36" s="15"/>
-      <c r="M36" s="26" t="s">
+      <c r="M36" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="N36" s="27"/>
-      <c r="O36" s="27"/>
-      <c r="P36" s="27"/>
-      <c r="R36" s="16"/>
-      <c r="S36" s="30"/>
+      <c r="N36" s="29"/>
+      <c r="O36" s="29"/>
+      <c r="P36" s="29"/>
+      <c r="Q36" s="12"/>
+      <c r="S36" s="16"/>
       <c r="U36" s="15" t="s">
         <v>0</v>
       </c>
       <c r="V36" s="15"/>
       <c r="W36" s="16"/>
-      <c r="X36" s="26" t="s">
+      <c r="X36" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="Y36" s="27"/>
-      <c r="Z36" s="27"/>
-      <c r="AA36" s="27"/>
+      <c r="Y36" s="29"/>
+      <c r="Z36" s="29"/>
+      <c r="AA36" s="29"/>
     </row>
     <row r="37" spans="2:28" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C37" s="11" t="s">
@@ -2381,10 +2391,10 @@
         <f>H37/$H$8%</f>
         <v>48.75346260387812</v>
       </c>
-      <c r="R37" s="14">
+      <c r="Q37" s="12"/>
+      <c r="S37" s="14">
         <v>1915</v>
       </c>
-      <c r="S37" s="30"/>
       <c r="U37" s="13"/>
       <c r="V37" s="13" t="s">
         <v>1</v>
@@ -2452,10 +2462,10 @@
         <f>H38/$H$8%</f>
         <v>60.110803324099727</v>
       </c>
-      <c r="R38" s="12">
+      <c r="Q38" s="12"/>
+      <c r="S38" s="12">
         <v>2123</v>
       </c>
-      <c r="S38" s="12"/>
       <c r="V38" s="11" t="s">
         <v>2</v>
       </c>
@@ -2508,7 +2518,7 @@
         <v>13</v>
       </c>
       <c r="N39" s="19"/>
-      <c r="R39" s="12"/>
+      <c r="Q39" s="12"/>
       <c r="S39" s="12"/>
       <c r="U39" s="11" t="s">
         <v>13</v>
@@ -2558,10 +2568,10 @@
         <f>H40/$H$8%</f>
         <v>33.795013850415515</v>
       </c>
-      <c r="R40" s="12">
+      <c r="Q40" s="12"/>
+      <c r="S40" s="12">
         <v>1429</v>
       </c>
-      <c r="S40" s="12"/>
       <c r="V40" s="11" t="s">
         <v>22</v>
       </c>
@@ -2628,10 +2638,10 @@
         <f t="shared" ref="P41:P42" si="10">H41/$H$8%</f>
         <v>37.950138504155127</v>
       </c>
-      <c r="R41" s="12">
+      <c r="Q41" s="12"/>
+      <c r="S41" s="12">
         <v>1297</v>
       </c>
-      <c r="S41" s="12"/>
       <c r="V41" s="11" t="s">
         <v>23</v>
       </c>
@@ -2698,10 +2708,10 @@
         <f t="shared" si="10"/>
         <v>37.119113573407205</v>
       </c>
-      <c r="R42" s="12">
+      <c r="Q42" s="12"/>
+      <c r="S42" s="12">
         <v>1312</v>
       </c>
-      <c r="S42" s="12"/>
       <c r="V42" s="11" t="s">
         <v>24</v>
       </c>
@@ -2755,7 +2765,7 @@
       </c>
       <c r="N43" s="19"/>
       <c r="O43" s="19"/>
-      <c r="R43" s="12"/>
+      <c r="Q43" s="12"/>
       <c r="S43" s="12"/>
       <c r="U43" s="11" t="s">
         <v>3</v>
@@ -2805,10 +2815,10 @@
         <f>H44/$H$8%</f>
         <v>32.963988919667592</v>
       </c>
-      <c r="R44" s="12">
+      <c r="Q44" s="12"/>
+      <c r="S44" s="12">
         <v>1210</v>
       </c>
-      <c r="S44" s="12"/>
       <c r="V44" s="11" t="s">
         <v>25</v>
       </c>
@@ -2875,10 +2885,10 @@
         <f t="shared" ref="P45" si="16">H45/$H$8%</f>
         <v>39.335180055401665</v>
       </c>
-      <c r="R45" s="12">
+      <c r="Q45" s="12"/>
+      <c r="S45" s="12">
         <v>1410</v>
       </c>
-      <c r="S45" s="12"/>
       <c r="V45" s="11" t="s">
         <v>4</v>
       </c>
@@ -2945,10 +2955,10 @@
         <f>H46/$H$8%</f>
         <v>9.418282548476455</v>
       </c>
-      <c r="R46" s="12">
+      <c r="Q46" s="12"/>
+      <c r="S46" s="12">
         <v>851</v>
       </c>
-      <c r="S46" s="12"/>
       <c r="V46" s="11" t="s">
         <v>5</v>
       </c>
@@ -3015,10 +3025,10 @@
         <f t="shared" ref="P47:P48" si="18">H47/$H$8%</f>
         <v>24.930747922437675</v>
       </c>
-      <c r="R47" s="12">
+      <c r="Q47" s="12"/>
+      <c r="S47" s="12">
         <v>410</v>
       </c>
-      <c r="S47" s="12"/>
       <c r="V47" s="11" t="s">
         <v>6</v>
       </c>
@@ -3085,10 +3095,10 @@
         <f t="shared" si="18"/>
         <v>2.21606648199446</v>
       </c>
-      <c r="R48" s="12">
+      <c r="Q48" s="12"/>
+      <c r="S48" s="12">
         <v>157</v>
       </c>
-      <c r="S48" s="12"/>
       <c r="V48" s="11" t="s">
         <v>14</v>
       </c>
@@ -3142,7 +3152,7 @@
       </c>
       <c r="N49" s="19"/>
       <c r="O49" s="19"/>
-      <c r="R49" s="12"/>
+      <c r="Q49" s="12"/>
       <c r="S49" s="12"/>
       <c r="U49" s="11" t="s">
         <v>7</v>
@@ -3192,10 +3202,10 @@
         <f>H50/$H$8%</f>
         <v>32.686980609418285</v>
       </c>
-      <c r="R50" s="12">
+      <c r="Q50" s="12"/>
+      <c r="S50" s="12">
         <v>1638</v>
       </c>
-      <c r="S50" s="12"/>
       <c r="V50" s="11" t="s">
         <v>15</v>
       </c>
@@ -3262,10 +3272,10 @@
         <f>H51/$H$8%</f>
         <v>17.72853185595568</v>
       </c>
-      <c r="R51" s="12">
+      <c r="Q51" s="12"/>
+      <c r="S51" s="12">
         <v>760</v>
       </c>
-      <c r="S51" s="12"/>
       <c r="V51" s="11" t="s">
         <v>17</v>
       </c>
@@ -3332,10 +3342,10 @@
         <f t="shared" ref="P52:P53" si="23">H52/$H$8%</f>
         <v>51.246537396121887</v>
       </c>
-      <c r="R52" s="12">
+      <c r="Q52" s="12"/>
+      <c r="S52" s="12">
         <v>1279</v>
       </c>
-      <c r="S52" s="12"/>
       <c r="V52" s="11" t="s">
         <v>16</v>
       </c>
@@ -3402,10 +3412,10 @@
         <f t="shared" si="23"/>
         <v>7.202216066481995</v>
       </c>
-      <c r="R53" s="12">
+      <c r="Q53" s="12"/>
+      <c r="S53" s="12">
         <v>361</v>
       </c>
-      <c r="S53" s="12"/>
       <c r="V53" s="11" t="s">
         <v>18</v>
       </c>
@@ -3459,7 +3469,7 @@
       </c>
       <c r="N54" s="19"/>
       <c r="O54" s="19"/>
-      <c r="R54" s="12"/>
+      <c r="Q54" s="12"/>
       <c r="S54" s="12"/>
       <c r="U54" s="11" t="s">
         <v>8</v>
@@ -3509,10 +3519,10 @@
         <f>H55/$H$8%</f>
         <v>14.681440443213297</v>
       </c>
-      <c r="R55" s="12">
+      <c r="Q55" s="12"/>
+      <c r="S55" s="12">
         <v>815</v>
       </c>
-      <c r="S55" s="12"/>
       <c r="V55" s="11" t="s">
         <v>19</v>
       </c>
@@ -3579,10 +3589,10 @@
         <f t="shared" ref="P56" si="28">H56/$H$8%</f>
         <v>44.044321329639892</v>
       </c>
-      <c r="R56" s="12">
+      <c r="Q56" s="12"/>
+      <c r="S56" s="12">
         <v>2152</v>
       </c>
-      <c r="S56" s="12"/>
       <c r="U56" s="15"/>
       <c r="V56" s="15" t="s">
         <v>21</v>
@@ -3651,11 +3661,11 @@
         <f>H57/$H$8%</f>
         <v>50.138504155124657</v>
       </c>
-      <c r="Q57" s="15"/>
-      <c r="R57" s="16">
+      <c r="Q57" s="12"/>
+      <c r="R57" s="15"/>
+      <c r="S57" s="16">
         <v>1071</v>
       </c>
-      <c r="S57" s="30"/>
       <c r="V57" s="11" t="s">
         <v>20</v>
       </c>
@@ -3839,7 +3849,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{77EDBE04-127B-4D30-9AC8-FAA1BDCAF585}">
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{0A184D5A-B882-4B3C-A16A-BC2831429DCD}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -3850,88 +3860,216 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Sheet1!M37:P37</xm:f>
-              <xm:sqref>Q37</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M38:P38</xm:f>
-              <xm:sqref>Q38</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M39:P39</xm:f>
-              <xm:sqref>Q39</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M40:P40</xm:f>
-              <xm:sqref>Q40</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M41:P41</xm:f>
-              <xm:sqref>Q41</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M42:P42</xm:f>
-              <xm:sqref>Q42</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M43:P43</xm:f>
-              <xm:sqref>Q43</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M44:P44</xm:f>
-              <xm:sqref>Q44</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M45:P45</xm:f>
-              <xm:sqref>Q45</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M46:P46</xm:f>
-              <xm:sqref>Q46</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M47:P47</xm:f>
-              <xm:sqref>Q47</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M48:P48</xm:f>
-              <xm:sqref>Q48</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M49:P49</xm:f>
-              <xm:sqref>Q49</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M50:P50</xm:f>
-              <xm:sqref>Q50</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M51:P51</xm:f>
-              <xm:sqref>Q51</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M52:P52</xm:f>
-              <xm:sqref>Q52</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M53:P53</xm:f>
-              <xm:sqref>Q53</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M54:P54</xm:f>
-              <xm:sqref>Q54</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M55:P55</xm:f>
-              <xm:sqref>Q55</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M56:P56</xm:f>
-              <xm:sqref>Q56</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M57:P57</xm:f>
-              <xm:sqref>Q57</xm:sqref>
+              <xm:f>Sheet1!M5:P5</xm:f>
+              <xm:sqref>R5</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M6:P6</xm:f>
+              <xm:sqref>R6</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M7:P7</xm:f>
+              <xm:sqref>R7</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M8:P8</xm:f>
+              <xm:sqref>R8</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M9:P9</xm:f>
+              <xm:sqref>R9</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M10:P10</xm:f>
+              <xm:sqref>R10</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M11:P11</xm:f>
+              <xm:sqref>R11</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M12:P12</xm:f>
+              <xm:sqref>R12</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M13:P13</xm:f>
+              <xm:sqref>R13</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M14:P14</xm:f>
+              <xm:sqref>R14</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M15:P15</xm:f>
+              <xm:sqref>R15</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M16:P16</xm:f>
+              <xm:sqref>R16</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M17:P17</xm:f>
+              <xm:sqref>R17</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M18:P18</xm:f>
+              <xm:sqref>R18</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M19:P19</xm:f>
+              <xm:sqref>R19</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M20:P20</xm:f>
+              <xm:sqref>R20</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M21:P21</xm:f>
+              <xm:sqref>R21</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M22:P22</xm:f>
+              <xm:sqref>R22</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M23:P23</xm:f>
+              <xm:sqref>R23</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M24:P24</xm:f>
+              <xm:sqref>R24</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M25:P25</xm:f>
+              <xm:sqref>R25</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M26:P26</xm:f>
+              <xm:sqref>R26</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M27:P27</xm:f>
+              <xm:sqref>R27</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M28:P28</xm:f>
+              <xm:sqref>R28</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M29:P29</xm:f>
+              <xm:sqref>R29</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{9309082F-C68D-4BE0-B6FB-5BBCC7127EC3}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Sheet1!X5:AA5</xm:f>
+              <xm:sqref>AC5</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!X6:AA6</xm:f>
+              <xm:sqref>AC6</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!X7:AA7</xm:f>
+              <xm:sqref>AC7</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!X8:AA8</xm:f>
+              <xm:sqref>AC8</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!X9:AA9</xm:f>
+              <xm:sqref>AC9</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!X10:AA10</xm:f>
+              <xm:sqref>AC10</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!X11:AA11</xm:f>
+              <xm:sqref>AC11</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!X12:AA12</xm:f>
+              <xm:sqref>AC12</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!X13:AA13</xm:f>
+              <xm:sqref>AC13</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!X14:AA14</xm:f>
+              <xm:sqref>AC14</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!X15:AA15</xm:f>
+              <xm:sqref>AC15</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!X16:AA16</xm:f>
+              <xm:sqref>AC16</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!X17:AA17</xm:f>
+              <xm:sqref>AC17</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!X18:AA18</xm:f>
+              <xm:sqref>AC18</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!X19:AA19</xm:f>
+              <xm:sqref>AC19</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!X20:AA20</xm:f>
+              <xm:sqref>AC20</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!X21:AA21</xm:f>
+              <xm:sqref>AC21</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!X22:AA22</xm:f>
+              <xm:sqref>AC22</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!X23:AA23</xm:f>
+              <xm:sqref>AC23</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!X24:AA24</xm:f>
+              <xm:sqref>AC24</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!X25:AA25</xm:f>
+              <xm:sqref>AC25</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!X26:AA26</xm:f>
+              <xm:sqref>AC26</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!X27:AA27</xm:f>
+              <xm:sqref>AC27</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!X28:AA28</xm:f>
+              <xm:sqref>AC28</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!X29:AA29</xm:f>
+              <xm:sqref>AC29</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -4031,7 +4169,7 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
-        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{9309082F-C68D-4BE0-B6FB-5BBCC7127EC3}">
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{77EDBE04-127B-4D30-9AC8-FAA1BDCAF585}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
           <x14:colorAxis rgb="FF000000"/>
@@ -4042,216 +4180,88 @@
           <x14:colorLow rgb="FFD00000"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>Sheet1!X5:AA5</xm:f>
-              <xm:sqref>AC5</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!X6:AA6</xm:f>
-              <xm:sqref>AC6</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!X7:AA7</xm:f>
-              <xm:sqref>AC7</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!X8:AA8</xm:f>
-              <xm:sqref>AC8</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!X9:AA9</xm:f>
-              <xm:sqref>AC9</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!X10:AA10</xm:f>
-              <xm:sqref>AC10</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!X11:AA11</xm:f>
-              <xm:sqref>AC11</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!X12:AA12</xm:f>
-              <xm:sqref>AC12</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!X13:AA13</xm:f>
-              <xm:sqref>AC13</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!X14:AA14</xm:f>
-              <xm:sqref>AC14</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!X15:AA15</xm:f>
-              <xm:sqref>AC15</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!X16:AA16</xm:f>
-              <xm:sqref>AC16</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!X17:AA17</xm:f>
-              <xm:sqref>AC17</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!X18:AA18</xm:f>
-              <xm:sqref>AC18</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!X19:AA19</xm:f>
-              <xm:sqref>AC19</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!X20:AA20</xm:f>
-              <xm:sqref>AC20</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!X21:AA21</xm:f>
-              <xm:sqref>AC21</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!X22:AA22</xm:f>
-              <xm:sqref>AC22</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!X23:AA23</xm:f>
-              <xm:sqref>AC23</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!X24:AA24</xm:f>
-              <xm:sqref>AC24</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!X25:AA25</xm:f>
-              <xm:sqref>AC25</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!X26:AA26</xm:f>
-              <xm:sqref>AC26</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!X27:AA27</xm:f>
-              <xm:sqref>AC27</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!X28:AA28</xm:f>
-              <xm:sqref>AC28</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!X29:AA29</xm:f>
-              <xm:sqref>AC29</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{0A184D5A-B882-4B3C-A16A-BC2831429DCD}">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>Sheet1!M5:P5</xm:f>
-              <xm:sqref>Q5</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M6:P6</xm:f>
-              <xm:sqref>Q6</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M7:P7</xm:f>
-              <xm:sqref>Q7</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M8:P8</xm:f>
-              <xm:sqref>Q8</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M9:P9</xm:f>
-              <xm:sqref>Q9</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M10:P10</xm:f>
-              <xm:sqref>Q10</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M11:P11</xm:f>
-              <xm:sqref>Q11</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M12:P12</xm:f>
-              <xm:sqref>Q12</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M13:P13</xm:f>
-              <xm:sqref>Q13</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M14:P14</xm:f>
-              <xm:sqref>Q14</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M15:P15</xm:f>
-              <xm:sqref>Q15</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M16:P16</xm:f>
-              <xm:sqref>Q16</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M17:P17</xm:f>
-              <xm:sqref>Q17</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M18:P18</xm:f>
-              <xm:sqref>Q18</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M19:P19</xm:f>
-              <xm:sqref>Q19</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M20:P20</xm:f>
-              <xm:sqref>Q20</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M21:P21</xm:f>
-              <xm:sqref>Q21</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M22:P22</xm:f>
-              <xm:sqref>Q22</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M23:P23</xm:f>
-              <xm:sqref>Q23</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M24:P24</xm:f>
-              <xm:sqref>Q24</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M25:P25</xm:f>
-              <xm:sqref>Q25</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M26:P26</xm:f>
-              <xm:sqref>Q26</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M27:P27</xm:f>
-              <xm:sqref>Q27</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M28:P28</xm:f>
-              <xm:sqref>Q28</xm:sqref>
-            </x14:sparkline>
-            <x14:sparkline>
-              <xm:f>Sheet1!M29:P29</xm:f>
-              <xm:sqref>Q29</xm:sqref>
+              <xm:f>Sheet1!M37:P37</xm:f>
+              <xm:sqref>R37</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M38:P38</xm:f>
+              <xm:sqref>R38</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M39:P39</xm:f>
+              <xm:sqref>R39</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M40:P40</xm:f>
+              <xm:sqref>R40</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M41:P41</xm:f>
+              <xm:sqref>R41</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M42:P42</xm:f>
+              <xm:sqref>R42</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M43:P43</xm:f>
+              <xm:sqref>R43</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M44:P44</xm:f>
+              <xm:sqref>R44</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M45:P45</xm:f>
+              <xm:sqref>R45</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M46:P46</xm:f>
+              <xm:sqref>R46</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M47:P47</xm:f>
+              <xm:sqref>R47</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M48:P48</xm:f>
+              <xm:sqref>R48</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M49:P49</xm:f>
+              <xm:sqref>R49</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M50:P50</xm:f>
+              <xm:sqref>R50</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M51:P51</xm:f>
+              <xm:sqref>R51</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M52:P52</xm:f>
+              <xm:sqref>R52</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M53:P53</xm:f>
+              <xm:sqref>R53</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M54:P54</xm:f>
+              <xm:sqref>R54</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M55:P55</xm:f>
+              <xm:sqref>R55</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M56:P56</xm:f>
+              <xm:sqref>R56</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Sheet1!M57:P57</xm:f>
+              <xm:sqref>R57</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>

</xml_diff>

<commit_message>
clean gh page repo
</commit_message>
<xml_diff>
--- a/eg_data/NHANES/PF/Waist2/Demog/Demog.xlsx
+++ b/eg_data/NHANES/PF/Waist2/Demog/Demog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadoh\OneDrive\Documents\GitHub\DietR\eg_data\NHANES\PF\Waist2\Demog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8970D3B9-80E3-4209-888D-330D9BAB3739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88FCD74-7AB6-4273-ABC3-EC83732AD1B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21450" yWindow="-2895" windowWidth="17940" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24525" yWindow="-3375" windowWidth="23670" windowHeight="13965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="38">
   <si>
     <t>Gender</t>
   </si>
@@ -204,7 +204,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,6 +252,19 @@
       <i/>
       <sz val="11"/>
       <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -307,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -397,6 +410,10 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -717,7 +734,7 @@
   <dimension ref="B1:AB102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,9 +752,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:28" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="18" t="s">
+      <c r="B1" s="43"/>
+      <c r="C1" s="43" t="s">
         <v>37</v>
       </c>
+      <c r="D1" s="43"/>
       <c r="U1" s="41"/>
       <c r="V1" s="41"/>
       <c r="W1" s="42"/>
@@ -902,20 +921,20 @@
         <v>1</v>
       </c>
       <c r="M6" s="6">
-        <f>E6/$E$42%</f>
-        <v>48.423913043478265</v>
+        <f>E6/E9%</f>
+        <v>48.982957669048922</v>
       </c>
       <c r="N6" s="6">
-        <f>F6/$F$42%</f>
-        <v>45.601436265709154</v>
+        <f t="shared" ref="N6:P6" si="0">F6/F9%</f>
+        <v>45.972850678733032</v>
       </c>
       <c r="O6" s="6">
-        <f>G6/$G$42%</f>
-        <v>45.42936288088643</v>
+        <f t="shared" si="0"/>
+        <v>45.555555555555557</v>
       </c>
       <c r="P6" s="6">
-        <f>H6/$H$42%</f>
-        <v>44.875346260387815</v>
+        <f t="shared" si="0"/>
+        <v>45.378151260504204</v>
       </c>
       <c r="Q6" s="1"/>
       <c r="S6" s="1">
@@ -975,20 +994,20 @@
         <v>2</v>
       </c>
       <c r="M7" s="6">
-        <f>E7/$E$42%</f>
-        <v>50.434782608695656</v>
+        <f>E7/E9%</f>
+        <v>51.017042330951071</v>
       </c>
       <c r="N7" s="6">
-        <f>F7/$F$42%</f>
-        <v>53.590664272890479</v>
+        <f>F7/F9%</f>
+        <v>54.027149321266968</v>
       </c>
       <c r="O7" s="6">
-        <f>G7/$G$42%</f>
-        <v>54.29362880886427</v>
+        <f t="shared" ref="O7:P7" si="1">G7/G9%</f>
+        <v>54.444444444444443</v>
       </c>
       <c r="P7" s="6">
-        <f>H7/$H$42%</f>
-        <v>54.016620498614962</v>
+        <f t="shared" si="1"/>
+        <v>54.621848739495803</v>
       </c>
       <c r="Q7" s="1"/>
       <c r="S7" s="1">
@@ -1018,7 +1037,7 @@
         <v>10.177453027139876</v>
       </c>
       <c r="AB7" s="38">
-        <f t="shared" ref="AB7" si="0">SUM(X7:AA7)</f>
+        <f t="shared" ref="AB7" si="2">SUM(X7:AA7)</f>
         <v>100</v>
       </c>
     </row>
@@ -1029,13 +1048,11 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="23"/>
-      <c r="L8" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="44"/>
+      <c r="N8" s="44"/>
+      <c r="O8" s="44"/>
+      <c r="P8" s="44"/>
       <c r="Q8" s="1"/>
       <c r="S8" s="1"/>
       <c r="X8" s="36"/>
@@ -1054,15 +1071,15 @@
         <v>1819</v>
       </c>
       <c r="F9" s="7">
-        <f t="shared" ref="F9:H9" si="1">SUM(F6:F7)</f>
+        <f t="shared" ref="F9:H9" si="3">SUM(F6:F7)</f>
         <v>1105</v>
       </c>
       <c r="G9" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>360</v>
       </c>
       <c r="H9" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>357</v>
       </c>
       <c r="I9" s="23">
@@ -1080,7 +1097,7 @@
         <v>13</v>
       </c>
       <c r="AB9" s="38">
-        <f t="shared" ref="AB9:AB12" si="2">SUM(X9:AA9)</f>
+        <f t="shared" ref="AB9:AB12" si="4">SUM(X9:AA9)</f>
         <v>0</v>
       </c>
     </row>
@@ -1108,20 +1125,20 @@
         <v>22</v>
       </c>
       <c r="M10" s="6">
-        <f>E10/$E$42%</f>
-        <v>38.641304347826093</v>
+        <f>E10/$E$14%</f>
+        <v>39.087410665200657</v>
       </c>
       <c r="N10" s="6">
-        <f>F10/$F$42%</f>
-        <v>33.393177737881508</v>
+        <f>F10/$F$14%</f>
+        <v>33.665158371040725</v>
       </c>
       <c r="O10" s="6">
-        <f>G10/$G$42%</f>
-        <v>31.855955678670362</v>
+        <f>G10/$G$14%</f>
+        <v>31.944444444444443</v>
       </c>
       <c r="P10" s="6">
-        <f>H10/$H$42%</f>
-        <v>31.301939058171747</v>
+        <f>H10/$H$14%</f>
+        <v>31.652661064425772</v>
       </c>
       <c r="Q10" s="1"/>
       <c r="S10" s="1">
@@ -1151,7 +1168,7 @@
         <v>8.6193745232646837</v>
       </c>
       <c r="AB10" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>99.999999999999986</v>
       </c>
     </row>
@@ -1180,20 +1197,20 @@
         <v>23</v>
       </c>
       <c r="M11" s="6">
-        <f>E11/$E$42%</f>
-        <v>30.489130434782609</v>
+        <f>E11/$E$14%</f>
+        <v>30.841121495327101</v>
       </c>
       <c r="N11" s="6">
-        <f>F11/$F$42%</f>
-        <v>32.585278276481148</v>
+        <f t="shared" ref="N11:N12" si="5">F11/$F$14%</f>
+        <v>32.850678733031671</v>
       </c>
       <c r="O11" s="6">
-        <f>G11/$G$42%</f>
-        <v>36.56509695290859</v>
+        <f t="shared" ref="O11:O12" si="6">G11/$G$14%</f>
+        <v>36.666666666666664</v>
       </c>
       <c r="P11" s="6">
-        <f>H11/$H$42%</f>
-        <v>34.34903047091413</v>
+        <f t="shared" ref="P11:P12" si="7">H11/$H$14%</f>
+        <v>34.733893557422974</v>
       </c>
       <c r="Q11" s="1"/>
       <c r="S11" s="1">
@@ -1223,7 +1240,7 @@
         <v>10.508474576271185</v>
       </c>
       <c r="AB11" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
     </row>
@@ -1252,20 +1269,20 @@
         <v>24</v>
       </c>
       <c r="M12" s="6">
-        <f>E12/$E$42%</f>
-        <v>29.728260869565219</v>
+        <f>E12/$E$14%</f>
+        <v>30.071467839472234</v>
       </c>
       <c r="N12" s="6">
-        <f>F12/$F$42%</f>
-        <v>33.213644524236983</v>
+        <f t="shared" si="5"/>
+        <v>33.484162895927597</v>
       </c>
       <c r="O12" s="6">
-        <f>G12/$G$42%</f>
-        <v>31.301939058171747</v>
+        <f t="shared" si="6"/>
+        <v>31.388888888888889</v>
       </c>
       <c r="P12" s="6">
-        <f>H12/$H$42%</f>
-        <v>33.2409972299169</v>
+        <f t="shared" si="7"/>
+        <v>33.613445378151262</v>
       </c>
       <c r="Q12" s="1"/>
       <c r="S12" s="1">
@@ -1295,7 +1312,7 @@
         <v>10.434782608695652</v>
       </c>
       <c r="AB12" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
     </row>
@@ -1307,10 +1324,10 @@
       <c r="H13" s="1"/>
       <c r="I13" s="23"/>
       <c r="L13" s="20"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
+      <c r="M13" s="44"/>
+      <c r="N13" s="44"/>
+      <c r="O13" s="44"/>
+      <c r="P13" s="44"/>
       <c r="Q13" s="1"/>
       <c r="S13" s="1"/>
       <c r="X13" s="36"/>
@@ -1329,15 +1346,15 @@
         <v>1819</v>
       </c>
       <c r="F14" s="7">
-        <f t="shared" ref="F14:H14" si="3">SUM(F10:F12)</f>
+        <f t="shared" ref="F14:H14" si="8">SUM(F10:F12)</f>
         <v>1105</v>
       </c>
       <c r="G14" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>360</v>
       </c>
       <c r="H14" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>357</v>
       </c>
       <c r="I14" s="22">
@@ -1356,7 +1373,7 @@
         <v>3</v>
       </c>
       <c r="AB14" s="38">
-        <f t="shared" ref="AB14:AB19" si="4">SUM(X14:AA14)</f>
+        <f t="shared" ref="AB14:AB19" si="9">SUM(X14:AA14)</f>
         <v>0</v>
       </c>
     </row>
@@ -1385,20 +1402,20 @@
         <v>25</v>
       </c>
       <c r="M15" s="6">
-        <f>E15/$E$42%</f>
-        <v>26.793478260869566</v>
+        <f>E15/$E$14%</f>
+        <v>27.102803738317753</v>
       </c>
       <c r="N15" s="6">
-        <f>F15/$F$42%</f>
-        <v>34.380610412926387</v>
+        <f>F15/$F$14%</f>
+        <v>34.660633484162894</v>
       </c>
       <c r="O15" s="6">
-        <f>G15/$G$42%</f>
-        <v>27.423822714681442</v>
+        <f>G15/$G$14%</f>
+        <v>27.5</v>
       </c>
       <c r="P15" s="6">
-        <f>H15/$H$42%</f>
-        <v>29.91689750692521</v>
+        <f>H15/$H$14%</f>
+        <v>30.252100840336137</v>
       </c>
       <c r="Q15" s="1"/>
       <c r="S15" s="1">
@@ -1428,7 +1445,7 @@
         <v>9.97229916897507</v>
       </c>
       <c r="AB15" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
     </row>
@@ -1457,20 +1474,20 @@
         <v>4</v>
       </c>
       <c r="M16" s="6">
-        <f>E16/$E$42%</f>
-        <v>36.141304347826093</v>
+        <f t="shared" ref="M16:M19" si="10">E16/$E$14%</f>
+        <v>36.558548653106101</v>
       </c>
       <c r="N16" s="6">
-        <f>F16/$F$42%</f>
-        <v>35.457809694793532</v>
+        <f t="shared" ref="N16" si="11">F16/$F$14%</f>
+        <v>35.74660633484163</v>
       </c>
       <c r="O16" s="6">
-        <f>G16/$G$42%</f>
-        <v>37.396121883656512</v>
+        <f t="shared" ref="O16" si="12">G16/$G$14%</f>
+        <v>37.5</v>
       </c>
       <c r="P16" s="6">
-        <f>H16/$H$42%</f>
-        <v>35.45706371191136</v>
+        <f t="shared" ref="P16" si="13">H16/$H$14%</f>
+        <v>35.854341736694678</v>
       </c>
       <c r="Q16" s="1"/>
       <c r="S16" s="1">
@@ -1500,7 +1517,7 @@
         <v>9.6749811035525326</v>
       </c>
       <c r="AB16" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
     </row>
@@ -1529,20 +1546,20 @@
         <v>5</v>
       </c>
       <c r="M17" s="6">
-        <f>E17/$E$42%</f>
-        <v>25.597826086956523</v>
+        <f t="shared" si="10"/>
+        <v>25.893347993402966</v>
       </c>
       <c r="N17" s="6">
-        <f>F17/$F$42%</f>
-        <v>17.235188509874327</v>
+        <f>F17/$F$14%</f>
+        <v>17.375565610859727</v>
       </c>
       <c r="O17" s="6">
-        <f>G17/$G$42%</f>
-        <v>12.742382271468145</v>
+        <f>G17/$G$14%</f>
+        <v>12.777777777777777</v>
       </c>
       <c r="P17" s="6">
-        <f>H17/$H$42%</f>
-        <v>9.1412742382271475</v>
+        <f>H17/$H$14%</f>
+        <v>9.2436974789915975</v>
       </c>
       <c r="Q17" s="1"/>
       <c r="S17" s="1">
@@ -1572,7 +1589,7 @@
         <v>4.44743935309973</v>
       </c>
       <c r="AB17" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
     </row>
@@ -1601,20 +1618,20 @@
         <v>6</v>
       </c>
       <c r="M18" s="6">
-        <f>E18/$E$42%</f>
-        <v>6.1413043478260878</v>
+        <f t="shared" si="10"/>
+        <v>6.2122045079714123</v>
       </c>
       <c r="N18" s="6">
-        <f>F18/$F$42%</f>
-        <v>8.2585278276481144</v>
+        <f t="shared" ref="N18:N19" si="14">F18/$F$14%</f>
+        <v>8.3257918552036188</v>
       </c>
       <c r="O18" s="6">
-        <f>G18/$G$42%</f>
-        <v>19.390581717451525</v>
+        <f t="shared" ref="O18:O19" si="15">G18/$G$14%</f>
+        <v>19.444444444444443</v>
       </c>
       <c r="P18" s="6">
-        <f>H18/$H$42%</f>
-        <v>22.714681440443215</v>
+        <f t="shared" ref="P18:P19" si="16">H18/$H$14%</f>
+        <v>22.969187675070028</v>
       </c>
       <c r="Q18" s="1"/>
       <c r="S18" s="1">
@@ -1644,7 +1661,7 @@
         <v>22.969187675070028</v>
       </c>
       <c r="AB18" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
     </row>
@@ -1673,20 +1690,20 @@
         <v>14</v>
       </c>
       <c r="M19" s="6">
-        <f>E19/$E$42%</f>
-        <v>4.1847826086956523</v>
+        <f t="shared" si="10"/>
+        <v>4.2330951072017591</v>
       </c>
       <c r="N19" s="6">
-        <f>F19/$F$42%</f>
-        <v>3.859964093357271</v>
+        <f t="shared" si="14"/>
+        <v>3.8914027149321266</v>
       </c>
       <c r="O19" s="6">
-        <f>G19/$G$42%</f>
-        <v>2.770083102493075</v>
+        <f t="shared" si="15"/>
+        <v>2.7777777777777777</v>
       </c>
       <c r="P19" s="6">
-        <f>H19/$H$42%</f>
-        <v>1.662049861495845</v>
+        <f t="shared" si="16"/>
+        <v>1.680672268907563</v>
       </c>
       <c r="Q19" s="1"/>
       <c r="S19" s="1">
@@ -1716,7 +1733,7 @@
         <v>4.4117647058823533</v>
       </c>
       <c r="AB19" s="38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
     </row>
@@ -1728,10 +1745,10 @@
       <c r="H20" s="1"/>
       <c r="I20" s="23"/>
       <c r="L20" s="20"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
+      <c r="M20" s="44"/>
+      <c r="N20" s="44"/>
+      <c r="O20" s="44"/>
+      <c r="P20" s="44"/>
       <c r="Q20" s="1"/>
       <c r="S20" s="1"/>
       <c r="X20" s="36"/>
@@ -1750,15 +1767,15 @@
         <v>1819</v>
       </c>
       <c r="F21" s="7">
-        <f t="shared" ref="F21:H21" si="5">SUM(F15:F19)</f>
+        <f t="shared" ref="F21:H21" si="17">SUM(F15:F19)</f>
         <v>1105</v>
       </c>
       <c r="G21" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="17"/>
         <v>360</v>
       </c>
       <c r="H21" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="17"/>
         <v>357</v>
       </c>
       <c r="I21" s="22">
@@ -1777,7 +1794,7 @@
         <v>7</v>
       </c>
       <c r="AB21" s="38">
-        <f t="shared" ref="AB21:AB24" si="6">SUM(X21:AA21)</f>
+        <f t="shared" ref="AB21:AB24" si="18">SUM(X21:AA21)</f>
         <v>0</v>
       </c>
     </row>
@@ -1806,20 +1823,20 @@
         <v>15</v>
       </c>
       <c r="M22" s="6">
-        <f>E22/$E$42%</f>
-        <v>48.750000000000007</v>
+        <f>E22/$E$14%</f>
+        <v>49.312809235843865</v>
       </c>
       <c r="N22" s="6">
-        <f>F22/$F$42%</f>
-        <v>43.985637342908433</v>
+        <f>F22/$F$14%</f>
+        <v>44.343891402714931</v>
       </c>
       <c r="O22" s="6">
-        <f>G22/$G$42%</f>
-        <v>32.409972299168977</v>
+        <f>G22/$G$14%</f>
+        <v>32.5</v>
       </c>
       <c r="P22" s="6">
-        <f>H22/$H$42%</f>
-        <v>32.13296398891967</v>
+        <f>H22/$H$14%</f>
+        <v>32.49299719887955</v>
       </c>
       <c r="Q22" s="1"/>
       <c r="S22" s="1">
@@ -1849,7 +1866,7 @@
         <v>7.1604938271604937</v>
       </c>
       <c r="AB22" s="38">
-        <f t="shared" si="6"/>
+        <f t="shared" si="18"/>
         <v>99.999999999999986</v>
       </c>
     </row>
@@ -1878,20 +1895,20 @@
         <v>17</v>
       </c>
       <c r="M23" s="6">
-        <f>E23/$E$42%</f>
-        <v>21.032608695652176</v>
+        <f t="shared" ref="M23:M24" si="19">E23/$E$14%</f>
+        <v>21.275426058273776</v>
       </c>
       <c r="N23" s="6">
-        <f>F23/$F$42%</f>
-        <v>20.017953321364452</v>
+        <f t="shared" ref="N23:N24" si="20">F23/$F$14%</f>
+        <v>20.180995475113122</v>
       </c>
       <c r="O23" s="6">
-        <f>G23/$G$42%</f>
-        <v>22.1606648199446</v>
+        <f t="shared" ref="O23:O24" si="21">G23/$G$14%</f>
+        <v>22.222222222222221</v>
       </c>
       <c r="P23" s="6">
-        <f>H23/$H$42%</f>
-        <v>17.72853185595568</v>
+        <f t="shared" ref="P23:P24" si="22">H23/$H$14%</f>
+        <v>17.927170868347339</v>
       </c>
       <c r="Q23" s="1"/>
       <c r="S23" s="1">
@@ -1921,7 +1938,7 @@
         <v>8.4880636604774526</v>
       </c>
       <c r="AB23" s="38">
-        <f t="shared" si="6"/>
+        <f t="shared" si="18"/>
         <v>100</v>
       </c>
     </row>
@@ -1950,20 +1967,20 @@
         <v>16</v>
       </c>
       <c r="M24" s="6">
-        <f>E24/$E$42%</f>
-        <v>29.076086956521742</v>
+        <f t="shared" si="19"/>
+        <v>29.411764705882351</v>
       </c>
       <c r="N24" s="6">
-        <f>F24/$F$42%</f>
-        <v>35.188509874326748</v>
+        <f t="shared" si="20"/>
+        <v>35.47511312217194</v>
       </c>
       <c r="O24" s="6">
-        <f>G24/$G$42%</f>
-        <v>45.152354570637122</v>
+        <f t="shared" si="21"/>
+        <v>45.277777777777779</v>
       </c>
       <c r="P24" s="6">
-        <f>H24/$H$42%</f>
-        <v>49.030470914127427</v>
+        <f t="shared" si="22"/>
+        <v>49.579831932773111</v>
       </c>
       <c r="Q24" s="1"/>
       <c r="S24" s="1">
@@ -1993,7 +2010,7 @@
         <v>13.970007892659828</v>
       </c>
       <c r="AB24" s="38">
-        <f t="shared" si="6"/>
+        <f t="shared" si="18"/>
         <v>99.999999999999986</v>
       </c>
     </row>
@@ -2005,10 +2022,10 @@
       <c r="H25" s="1"/>
       <c r="I25" s="23"/>
       <c r="L25" s="20"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
-      <c r="P25" s="6"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="44"/>
+      <c r="O25" s="44"/>
+      <c r="P25" s="44"/>
       <c r="Q25" s="1"/>
       <c r="S25" s="1"/>
       <c r="X25" s="36"/>
@@ -2054,7 +2071,7 @@
         <v>8</v>
       </c>
       <c r="AB26" s="38">
-        <f t="shared" ref="AB26:AB28" si="7">SUM(X26:AA26)</f>
+        <f t="shared" ref="AB26:AB28" si="23">SUM(X26:AA26)</f>
         <v>0</v>
       </c>
     </row>
@@ -2063,7 +2080,7 @@
         <v>19</v>
       </c>
       <c r="D27" s="7">
-        <f t="shared" ref="D27:D28" si="8">SUM(E27:H27)</f>
+        <f t="shared" ref="D27:D28" si="24">SUM(E27:H27)</f>
         <v>712</v>
       </c>
       <c r="E27">
@@ -2083,20 +2100,20 @@
         <v>19</v>
       </c>
       <c r="M27" s="6">
-        <f>E27/$E$42%</f>
-        <v>21.25</v>
+        <f>E27/$E$14%</f>
+        <v>21.495327102803738</v>
       </c>
       <c r="N27" s="6">
-        <f>F27/$F$42%</f>
-        <v>20.466786355475762</v>
+        <f>F27/$F$14%</f>
+        <v>20.633484162895925</v>
       </c>
       <c r="O27" s="6">
-        <f>G27/$G$42%</f>
-        <v>12.742382271468145</v>
+        <f>G27/$G$14%</f>
+        <v>12.777777777777777</v>
       </c>
       <c r="P27" s="6">
-        <f>H27/$H$42%</f>
-        <v>13.019390581717452</v>
+        <f>H27/$H$14%</f>
+        <v>13.165266106442578</v>
       </c>
       <c r="Q27" s="1"/>
       <c r="S27" s="1">
@@ -2126,7 +2143,7 @@
         <v>6.6011235955056176</v>
       </c>
       <c r="AB27" s="38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="23"/>
         <v>100</v>
       </c>
     </row>
@@ -2135,7 +2152,7 @@
         <v>21</v>
       </c>
       <c r="D28" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="24"/>
         <v>1948</v>
       </c>
       <c r="E28">
@@ -2155,20 +2172,20 @@
         <v>21</v>
       </c>
       <c r="M28" s="6">
-        <f>E28/$E$42%</f>
-        <v>57.989130434782616</v>
+        <f t="shared" ref="M28:M29" si="25">E28/$E$14%</f>
+        <v>58.658603628367231</v>
       </c>
       <c r="N28" s="6">
-        <f>F28/$F$42%</f>
-        <v>51.25673249551167</v>
+        <f t="shared" ref="N28" si="26">F28/$F$14%</f>
+        <v>51.674208144796374</v>
       </c>
       <c r="O28" s="6">
-        <f>G28/$G$42%</f>
-        <v>46.260387811634352</v>
+        <f t="shared" ref="O28:O29" si="27">G28/$G$14%</f>
+        <v>46.388888888888886</v>
       </c>
       <c r="P28" s="6">
-        <f>H28/$H$42%</f>
-        <v>39.612188365650972</v>
+        <f t="shared" ref="P28:P29" si="28">H28/$H$14%</f>
+        <v>40.056022408963585</v>
       </c>
       <c r="Q28" s="1"/>
       <c r="S28" s="1">
@@ -2199,7 +2216,7 @@
         <v>7.3408624229979473</v>
       </c>
       <c r="AB28" s="38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="23"/>
         <v>100</v>
       </c>
     </row>
@@ -2228,20 +2245,20 @@
         <v>20</v>
       </c>
       <c r="M29" s="6">
-        <f>E29/$E$42%</f>
-        <v>19.619565217391305</v>
+        <f t="shared" si="25"/>
+        <v>19.846069268829027</v>
       </c>
       <c r="N29" s="6">
-        <f>F29/$F$42%</f>
-        <v>27.468581687612208</v>
+        <f>F29/$F$14%</f>
+        <v>27.69230769230769</v>
       </c>
       <c r="O29" s="6">
-        <f>G29/$G$42%</f>
-        <v>40.720221606648202</v>
+        <f t="shared" si="27"/>
+        <v>40.833333333333336</v>
       </c>
       <c r="P29" s="6">
-        <f>H29/$H$42%</f>
-        <v>46.260387811634352</v>
+        <f t="shared" si="28"/>
+        <v>46.778711484593842</v>
       </c>
       <c r="Q29" s="1"/>
       <c r="S29" s="1">
@@ -2281,10 +2298,10 @@
       <c r="H30" s="1"/>
       <c r="I30" s="23"/>
       <c r="L30" s="20"/>
-      <c r="M30" s="6"/>
-      <c r="N30" s="6"/>
-      <c r="O30" s="6"/>
-      <c r="P30" s="6"/>
+      <c r="M30" s="44"/>
+      <c r="N30" s="44"/>
+      <c r="O30" s="44"/>
+      <c r="P30" s="44"/>
       <c r="Q30" s="1"/>
       <c r="S30" s="1"/>
       <c r="X30" s="36"/>
@@ -2300,15 +2317,15 @@
         <v>1819</v>
       </c>
       <c r="F31" s="7">
-        <f t="shared" ref="F31:H31" si="9">SUM(F27:F29)</f>
+        <f t="shared" ref="F31:H31" si="29">SUM(F27:F29)</f>
         <v>1105</v>
       </c>
       <c r="G31" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="29"/>
         <v>360</v>
       </c>
       <c r="H31" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="29"/>
         <v>357</v>
       </c>
       <c r="I31" s="23"/>
@@ -2616,7 +2633,7 @@
         <v>9.7876747799067836</v>
       </c>
       <c r="AB40" s="38">
-        <f t="shared" ref="AB40:AB61" si="10">SUM(X40:AA40)</f>
+        <f t="shared" ref="AB40:AB61" si="30">SUM(X40:AA40)</f>
         <v>100</v>
       </c>
     </row>
@@ -2653,15 +2670,15 @@
         <v>1840</v>
       </c>
       <c r="F42" s="35">
-        <f t="shared" ref="F42:H42" si="11">SUM(F39:F40)</f>
+        <f t="shared" ref="F42:H42" si="31">SUM(F39:F40)</f>
         <v>1114</v>
       </c>
       <c r="G42" s="35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="31"/>
         <v>361</v>
       </c>
       <c r="H42" s="35">
-        <f t="shared" si="11"/>
+        <f t="shared" si="31"/>
         <v>361</v>
       </c>
       <c r="I42" s="34">
@@ -2680,7 +2697,7 @@
       </c>
       <c r="W42" s="27"/>
       <c r="AB42" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
     </row>
@@ -2752,7 +2769,7 @@
         <v>9.2424242424242422</v>
       </c>
       <c r="AB43" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="30"/>
         <v>100</v>
       </c>
     </row>
@@ -2824,7 +2841,7 @@
         <v>10</v>
       </c>
       <c r="AB44" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="30"/>
         <v>100</v>
       </c>
     </row>
@@ -2896,7 +2913,7 @@
         <v>10.291595197255575</v>
       </c>
       <c r="AB45" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="30"/>
         <v>100</v>
       </c>
     </row>
@@ -2931,15 +2948,15 @@
         <v>1840</v>
       </c>
       <c r="F47" s="35">
-        <f t="shared" ref="F47:H47" si="12">SUM(F43:F45)</f>
+        <f t="shared" ref="F47:H47" si="32">SUM(F43:F45)</f>
         <v>1114</v>
       </c>
       <c r="G47" s="35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="32"/>
         <v>361</v>
       </c>
       <c r="H47" s="35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="32"/>
         <v>361</v>
       </c>
       <c r="I47" s="34">
@@ -2959,7 +2976,7 @@
       </c>
       <c r="W47" s="27"/>
       <c r="AB47" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
     </row>
@@ -3031,7 +3048,7 @@
         <v>10.714285714285714</v>
       </c>
       <c r="AB48" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="30"/>
         <v>100</v>
       </c>
     </row>
@@ -3103,7 +3120,7 @@
         <v>9.7891566265060241</v>
       </c>
       <c r="AB49" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="30"/>
         <v>100.00000000000001</v>
       </c>
     </row>
@@ -3175,7 +3192,7 @@
         <v>4.5152722443559101</v>
       </c>
       <c r="AB50" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="30"/>
         <v>100</v>
       </c>
     </row>
@@ -3247,7 +3264,7 @@
         <v>20.385674931129476</v>
       </c>
       <c r="AB51" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="30"/>
         <v>100</v>
       </c>
     </row>
@@ -3319,7 +3336,7 @@
         <v>4.2857142857142856</v>
       </c>
       <c r="AB52" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="30"/>
         <v>100.00000000000001</v>
       </c>
     </row>
@@ -3354,15 +3371,15 @@
         <v>1840</v>
       </c>
       <c r="F54" s="35">
-        <f t="shared" ref="F54:H54" si="13">SUM(F48:F52)</f>
+        <f t="shared" ref="F54:H54" si="33">SUM(F48:F52)</f>
         <v>1114</v>
       </c>
       <c r="G54" s="35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="33"/>
         <v>361</v>
       </c>
       <c r="H54" s="35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="33"/>
         <v>361</v>
       </c>
       <c r="I54" s="34">
@@ -3382,7 +3399,7 @@
       </c>
       <c r="W54" s="27"/>
       <c r="AB54" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
     </row>
@@ -3454,7 +3471,7 @@
         <v>7.57020757020757</v>
       </c>
       <c r="AB55" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="30"/>
         <v>100</v>
       </c>
     </row>
@@ -3526,7 +3543,7 @@
         <v>7.8947368421052628</v>
       </c>
       <c r="AB56" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="30"/>
         <v>100</v>
       </c>
     </row>
@@ -3598,7 +3615,7 @@
         <v>13.849765258215962</v>
       </c>
       <c r="AB57" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="30"/>
         <v>100</v>
       </c>
     </row>
@@ -3661,7 +3678,7 @@
       </c>
       <c r="W59" s="27"/>
       <c r="AB59" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
     </row>
@@ -3670,7 +3687,7 @@
         <v>19</v>
       </c>
       <c r="D60" s="35">
-        <f t="shared" ref="D60:D61" si="14">SUM(E60:H60)</f>
+        <f t="shared" ref="D60:D61" si="34">SUM(E60:H60)</f>
         <v>720</v>
       </c>
       <c r="E60" s="26">
@@ -3733,7 +3750,7 @@
         <v>7.083333333333333</v>
       </c>
       <c r="AB60" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="30"/>
         <v>100</v>
       </c>
     </row>
@@ -3742,7 +3759,7 @@
         <v>21</v>
       </c>
       <c r="D61" s="35">
-        <f t="shared" si="14"/>
+        <f t="shared" si="34"/>
         <v>1965</v>
       </c>
       <c r="E61" s="26">
@@ -3806,7 +3823,7 @@
         <v>7.7353689567430024</v>
       </c>
       <c r="AB61" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="30"/>
         <v>100</v>
       </c>
     </row>
@@ -3908,15 +3925,15 @@
         <v>1840</v>
       </c>
       <c r="F64" s="35">
-        <f t="shared" ref="F64:H64" si="15">SUM(F60:F62)</f>
+        <f t="shared" ref="F64:H64" si="35">SUM(F60:F62)</f>
         <v>1114</v>
       </c>
       <c r="G64" s="35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="35"/>
         <v>361</v>
       </c>
       <c r="H64" s="35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="35"/>
         <v>361</v>
       </c>
       <c r="I64" s="34"/>
@@ -4036,12 +4053,12 @@
         <v>0</v>
       </c>
       <c r="L70" s="12"/>
-      <c r="M70" s="43" t="s">
+      <c r="M70" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="N70" s="44"/>
-      <c r="O70" s="44"/>
-      <c r="P70" s="44"/>
+      <c r="N70" s="46"/>
+      <c r="O70" s="46"/>
+      <c r="P70" s="46"/>
       <c r="Q70" s="9"/>
       <c r="S70" s="13"/>
       <c r="U70" s="30" t="s">
@@ -4049,12 +4066,12 @@
       </c>
       <c r="V70" s="30"/>
       <c r="W70" s="32"/>
-      <c r="X70" s="45" t="s">
+      <c r="X70" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="Y70" s="46"/>
-      <c r="Z70" s="46"/>
-      <c r="AA70" s="46"/>
+      <c r="Y70" s="48"/>
+      <c r="Z70" s="48"/>
+      <c r="AA70" s="48"/>
       <c r="AB70" s="26"/>
     </row>
     <row r="71" spans="2:28" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -4196,7 +4213,7 @@
         <v>10.221384832783796</v>
       </c>
       <c r="AB72" s="38">
-        <f t="shared" ref="AB72:AB90" si="16">SUM(X72:AA72)</f>
+        <f t="shared" ref="AB72:AB90" si="36">SUM(X72:AA72)</f>
         <v>100.00000000000001</v>
       </c>
     </row>
@@ -4210,15 +4227,15 @@
         <v>2012</v>
       </c>
       <c r="F73" s="14">
-        <f t="shared" ref="F73:H73" si="17">SUM(F71:F72)</f>
+        <f t="shared" ref="F73:H73" si="37">SUM(F71:F72)</f>
         <v>1246</v>
       </c>
       <c r="G73" s="14">
-        <f t="shared" si="17"/>
+        <f t="shared" si="37"/>
         <v>387</v>
       </c>
       <c r="H73" s="14">
-        <f t="shared" si="17"/>
+        <f t="shared" si="37"/>
         <v>393</v>
       </c>
       <c r="K73" s="8" t="s">
@@ -4237,7 +4254,7 @@
       <c r="Z73" s="26"/>
       <c r="AA73" s="26"/>
       <c r="AB73" s="38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
     </row>
@@ -4269,7 +4286,7 @@
         <v>42.010869565217398</v>
       </c>
       <c r="N74" s="16">
-        <f t="shared" ref="N74:N76" si="18">F74/$F$42%</f>
+        <f t="shared" ref="N74:N76" si="38">F74/$F$42%</f>
         <v>36.714542190305202</v>
       </c>
       <c r="O74" s="16">
@@ -4308,7 +4325,7 @@
         <v>8.5374387683694888</v>
       </c>
       <c r="AB74" s="38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="36"/>
         <v>100</v>
       </c>
     </row>
@@ -4336,11 +4353,11 @@
         <v>23</v>
       </c>
       <c r="M75" s="16">
-        <f t="shared" ref="M75" si="19">E75/$E$42%</f>
+        <f t="shared" ref="M75" si="39">E75/$E$42%</f>
         <v>33.423913043478265</v>
       </c>
       <c r="N75" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="38"/>
         <v>36.714542190305202</v>
       </c>
       <c r="O75" s="16">
@@ -4348,7 +4365,7 @@
         <v>37.67313019390582</v>
       </c>
       <c r="P75" s="16">
-        <f t="shared" ref="P75:P76" si="20">H75/$H$42%</f>
+        <f t="shared" ref="P75:P76" si="40">H75/$H$42%</f>
         <v>37.950138504155127</v>
       </c>
       <c r="Q75" s="9"/>
@@ -4379,7 +4396,7 @@
         <v>10.562837316885119</v>
       </c>
       <c r="AB75" s="38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="36"/>
         <v>100.00000000000001</v>
       </c>
     </row>
@@ -4411,15 +4428,15 @@
         <v>33.913043478260875</v>
       </c>
       <c r="N76" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="38"/>
         <v>38.420107719928183</v>
       </c>
       <c r="O76" s="16">
-        <f t="shared" ref="O76" si="21">G76/$G$42%</f>
+        <f t="shared" ref="O76" si="41">G76/$G$42%</f>
         <v>34.903047091412745</v>
       </c>
       <c r="P76" s="16">
-        <f t="shared" si="20"/>
+        <f t="shared" si="40"/>
         <v>37.119113573407205</v>
       </c>
       <c r="Q76" s="9"/>
@@ -4450,7 +4467,7 @@
         <v>10.213414634146341</v>
       </c>
       <c r="AB76" s="38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="36"/>
         <v>100.00000000000001</v>
       </c>
     </row>
@@ -4464,15 +4481,15 @@
         <v>2012</v>
       </c>
       <c r="F77" s="14">
-        <f t="shared" ref="F77:H77" si="22">SUM(F74:F76)</f>
+        <f t="shared" ref="F77:H77" si="42">SUM(F74:F76)</f>
         <v>1246</v>
       </c>
       <c r="G77" s="14">
-        <f t="shared" si="22"/>
+        <f t="shared" si="42"/>
         <v>387</v>
       </c>
       <c r="H77" s="14">
-        <f t="shared" si="22"/>
+        <f t="shared" si="42"/>
         <v>393</v>
       </c>
       <c r="K77" s="8" t="s">
@@ -4492,7 +4509,7 @@
       <c r="Z77" s="26"/>
       <c r="AA77" s="26"/>
       <c r="AB77" s="38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
     </row>
@@ -4524,11 +4541,11 @@
         <v>29.619565217391308</v>
       </c>
       <c r="N78" s="16">
-        <f t="shared" ref="N78:N82" si="23">F78/$F$42%</f>
+        <f t="shared" ref="N78:N82" si="43">F78/$F$42%</f>
         <v>39.317773788150809</v>
       </c>
       <c r="O78" s="16">
-        <f t="shared" ref="O78:O82" si="24">G78/$G$42%</f>
+        <f t="shared" ref="O78:O82" si="44">G78/$G$42%</f>
         <v>29.91689750692521</v>
       </c>
       <c r="P78" s="16">
@@ -4563,7 +4580,7 @@
         <v>9.8347107438016526</v>
       </c>
       <c r="AB78" s="38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="36"/>
         <v>100</v>
       </c>
     </row>
@@ -4591,19 +4608,19 @@
         <v>4</v>
       </c>
       <c r="M79" s="16">
-        <f t="shared" ref="M79" si="25">E79/$E$42%</f>
+        <f t="shared" ref="M79" si="45">E79/$E$42%</f>
         <v>38.478260869565219</v>
       </c>
       <c r="N79" s="16">
-        <f t="shared" si="23"/>
+        <f t="shared" si="43"/>
         <v>38.240574506283657</v>
       </c>
       <c r="O79" s="16">
-        <f t="shared" si="24"/>
+        <f t="shared" si="44"/>
         <v>37.119113573407205</v>
       </c>
       <c r="P79" s="16">
-        <f t="shared" ref="P79" si="26">H79/$H$42%</f>
+        <f t="shared" ref="P79" si="46">H79/$H$42%</f>
         <v>39.335180055401665</v>
       </c>
       <c r="Q79" s="9"/>
@@ -4634,7 +4651,7 @@
         <v>10.070921985815604</v>
       </c>
       <c r="AB79" s="38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="36"/>
         <v>100</v>
       </c>
     </row>
@@ -4666,11 +4683,11 @@
         <v>29.347826086956523</v>
       </c>
       <c r="N80" s="16">
-        <f t="shared" si="23"/>
+        <f t="shared" si="43"/>
         <v>20.017953321364452</v>
       </c>
       <c r="O80" s="16">
-        <f t="shared" si="24"/>
+        <f t="shared" si="44"/>
         <v>14.958448753462605</v>
       </c>
       <c r="P80" s="16">
@@ -4705,7 +4722,7 @@
         <v>3.9952996474735603</v>
       </c>
       <c r="AB80" s="38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="36"/>
         <v>100</v>
       </c>
     </row>
@@ -4733,19 +4750,19 @@
         <v>6</v>
       </c>
       <c r="M81" s="16">
-        <f t="shared" ref="M81" si="27">E81/$E$42%</f>
+        <f t="shared" ref="M81" si="47">E81/$E$42%</f>
         <v>7.0652173913043486</v>
       </c>
       <c r="N81" s="16">
-        <f t="shared" si="23"/>
+        <f t="shared" si="43"/>
         <v>9.9640933572710946</v>
       </c>
       <c r="O81" s="16">
-        <f t="shared" si="24"/>
+        <f t="shared" si="44"/>
         <v>21.883656509695292</v>
       </c>
       <c r="P81" s="16">
-        <f t="shared" ref="P81:P82" si="28">H81/$H$42%</f>
+        <f t="shared" ref="P81:P82" si="48">H81/$H$42%</f>
         <v>24.930747922437675</v>
       </c>
       <c r="Q81" s="9"/>
@@ -4776,7 +4793,7 @@
         <v>21.951219512195124</v>
       </c>
       <c r="AB81" s="38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="36"/>
         <v>100</v>
       </c>
     </row>
@@ -4808,15 +4825,15 @@
         <v>4.8369565217391308</v>
       </c>
       <c r="N82" s="16">
-        <f t="shared" si="23"/>
+        <f t="shared" si="43"/>
         <v>4.3087971274685817</v>
       </c>
       <c r="O82" s="16">
-        <f t="shared" si="24"/>
+        <f t="shared" si="44"/>
         <v>3.32409972299169</v>
       </c>
       <c r="P82" s="16">
-        <f t="shared" si="28"/>
+        <f t="shared" si="48"/>
         <v>2.21606648199446</v>
       </c>
       <c r="Q82" s="9"/>
@@ -4847,7 +4864,7 @@
         <v>5.095541401273886</v>
       </c>
       <c r="AB82" s="38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="36"/>
         <v>100</v>
       </c>
     </row>
@@ -4861,15 +4878,15 @@
         <v>2012</v>
       </c>
       <c r="F83" s="14">
-        <f t="shared" ref="F83:H83" si="29">SUM(F78:F82)</f>
+        <f t="shared" ref="F83:H83" si="49">SUM(F78:F82)</f>
         <v>1246</v>
       </c>
       <c r="G83" s="14">
-        <f t="shared" si="29"/>
+        <f t="shared" si="49"/>
         <v>387</v>
       </c>
       <c r="H83" s="14">
-        <f t="shared" si="29"/>
+        <f t="shared" si="49"/>
         <v>393</v>
       </c>
       <c r="K83" s="8" t="s">
@@ -4889,7 +4906,7 @@
       <c r="Z83" s="26"/>
       <c r="AA83" s="26"/>
       <c r="AB83" s="38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
     </row>
@@ -4921,11 +4938,11 @@
         <v>49.402173913043484</v>
       </c>
       <c r="N84" s="16">
-        <f t="shared" ref="N84:N87" si="30">F84/$F$42%</f>
+        <f t="shared" ref="N84:N87" si="50">F84/$F$42%</f>
         <v>44.524236983842009</v>
       </c>
       <c r="O84" s="16">
-        <f t="shared" ref="O84:O87" si="31">G84/$G$42%</f>
+        <f t="shared" ref="O84:O87" si="51">G84/$G$42%</f>
         <v>31.855955678670362</v>
       </c>
       <c r="P84" s="16">
@@ -4960,7 +4977,7 @@
         <v>7.2039072039072032</v>
       </c>
       <c r="AB84" s="38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="36"/>
         <v>100</v>
       </c>
     </row>
@@ -4992,11 +5009,11 @@
         <v>21.358695652173914</v>
       </c>
       <c r="N85" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="50"/>
         <v>20.017953321364452</v>
       </c>
       <c r="O85" s="16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="51"/>
         <v>22.1606648199446</v>
       </c>
       <c r="P85" s="16">
@@ -5031,7 +5048,7 @@
         <v>8.4210526315789469</v>
       </c>
       <c r="AB85" s="38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="36"/>
         <v>100</v>
       </c>
     </row>
@@ -5059,19 +5076,19 @@
         <v>16</v>
       </c>
       <c r="M86" s="16">
-        <f t="shared" ref="M86" si="32">E86/$E$42%</f>
+        <f t="shared" ref="M86" si="52">E86/$E$42%</f>
         <v>29.239130434782609</v>
       </c>
       <c r="N86" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="50"/>
         <v>35.457809694793532</v>
       </c>
       <c r="O86" s="16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="51"/>
         <v>44.598337950138507</v>
       </c>
       <c r="P86" s="16">
-        <f t="shared" ref="P86:P87" si="33">H86/$H$42%</f>
+        <f t="shared" ref="P86:P87" si="53">H86/$H$42%</f>
         <v>51.246537396121887</v>
       </c>
       <c r="Q86" s="9"/>
@@ -5102,7 +5119,7 @@
         <v>14.464425332290853</v>
       </c>
       <c r="AB86" s="38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="36"/>
         <v>100.00000000000001</v>
       </c>
     </row>
@@ -5134,15 +5151,15 @@
         <v>9.3478260869565233</v>
       </c>
       <c r="N87" s="16">
-        <f t="shared" si="30"/>
+        <f t="shared" si="50"/>
         <v>11.849192100538598</v>
       </c>
       <c r="O87" s="16">
-        <f t="shared" si="31"/>
+        <f t="shared" si="51"/>
         <v>8.5872576177285325</v>
       </c>
       <c r="P87" s="16">
-        <f t="shared" si="33"/>
+        <f t="shared" si="53"/>
         <v>7.202216066481995</v>
       </c>
       <c r="Q87" s="9"/>
@@ -5173,7 +5190,7 @@
         <v>7.202216066481995</v>
       </c>
       <c r="AB87" s="38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="36"/>
         <v>100.00000000000001</v>
       </c>
     </row>
@@ -5187,15 +5204,15 @@
         <v>2012</v>
       </c>
       <c r="F88" s="14">
-        <f t="shared" ref="F88:H88" si="34">SUM(F84:F87)</f>
+        <f t="shared" ref="F88:H88" si="54">SUM(F84:F87)</f>
         <v>1246</v>
       </c>
       <c r="G88" s="14">
-        <f t="shared" si="34"/>
+        <f t="shared" si="54"/>
         <v>387</v>
       </c>
       <c r="H88" s="14">
-        <f t="shared" si="34"/>
+        <f t="shared" si="54"/>
         <v>393</v>
       </c>
       <c r="K88" s="8" t="s">
@@ -5215,7 +5232,7 @@
       <c r="Z88" s="26"/>
       <c r="AA88" s="26"/>
       <c r="AB88" s="38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
     </row>
@@ -5224,7 +5241,7 @@
         <v>19</v>
       </c>
       <c r="D89" s="14">
-        <f t="shared" ref="D89:D90" si="35">SUM(E89:H89)</f>
+        <f t="shared" ref="D89:D90" si="55">SUM(E89:H89)</f>
         <v>815</v>
       </c>
       <c r="E89" s="9">
@@ -5247,11 +5264,11 @@
         <v>24.510869565217394</v>
       </c>
       <c r="N89" s="16">
-        <f t="shared" ref="N89:N90" si="36">F89/$F$42%</f>
+        <f t="shared" ref="N89:N90" si="56">F89/$F$42%</f>
         <v>23.159784560143624</v>
       </c>
       <c r="O89" s="16">
-        <f t="shared" ref="O89:O90" si="37">G89/$G$42%</f>
+        <f t="shared" ref="O89:O90" si="57">G89/$G$42%</f>
         <v>14.681440443213297</v>
       </c>
       <c r="P89" s="16">
@@ -5286,7 +5303,7 @@
         <v>6.5030674846625764</v>
       </c>
       <c r="AB89" s="38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="36"/>
         <v>100.00000000000001</v>
       </c>
     </row>
@@ -5295,7 +5312,7 @@
         <v>21</v>
       </c>
       <c r="D90" s="14">
-        <f t="shared" si="35"/>
+        <f t="shared" si="55"/>
         <v>2152</v>
       </c>
       <c r="E90" s="9">
@@ -5318,15 +5335,15 @@
         <v>63.695652173913047</v>
       </c>
       <c r="N90" s="16">
-        <f t="shared" si="36"/>
+        <f t="shared" si="56"/>
         <v>57.809694793536799</v>
       </c>
       <c r="O90" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="57"/>
         <v>49.030470914127427</v>
       </c>
       <c r="P90" s="16">
-        <f t="shared" ref="P90" si="38">H90/$H$42%</f>
+        <f t="shared" ref="P90" si="58">H90/$H$42%</f>
         <v>44.044321329639892</v>
       </c>
       <c r="Q90" s="9"/>
@@ -5357,7 +5374,7 @@
         <v>7.3884758364312271</v>
       </c>
       <c r="AB90" s="38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="36"/>
         <v>100</v>
       </c>
     </row>
@@ -5441,15 +5458,15 @@
         <v>2012</v>
       </c>
       <c r="F92" s="14">
-        <f t="shared" ref="F92:H92" si="39">SUM(F89:F91)</f>
+        <f t="shared" ref="F92:H92" si="59">SUM(F89:F91)</f>
         <v>1246</v>
       </c>
       <c r="G92" s="14">
-        <f t="shared" si="39"/>
+        <f t="shared" si="59"/>
         <v>387</v>
       </c>
       <c r="H92" s="14">
-        <f t="shared" si="39"/>
+        <f t="shared" si="59"/>
         <v>393</v>
       </c>
       <c r="U92" s="26"/>

</xml_diff>